<commit_message>
SVN Revision #6786 by jireh360       Merged revision(s) from branches/CBECC-Com_EnergyPlus94
</commit_message>
<xml_diff>
--- a/Documentation/T24N/T24R_CentralHPWHCompressors.xlsx
+++ b/Documentation/T24N/T24R_CentralHPWHCompressors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\svn-CEC\SF_CBECC-Res\trunk\RulesetDev\Rulesets\CA Res\Rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3A2246-CEB1-478E-8AEC-1CB4B5505087}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237A9B4C-7BB9-46CA-B308-5073F6A644BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="1470" windowWidth="24315" windowHeight="12945" xr2:uid="{06DD2E85-E74E-41DF-AAE4-37E8BABFD5C8}"/>
+    <workbookView xWindow="2730" yWindow="1575" windowWidth="24210" windowHeight="12930" xr2:uid="{06DD2E85-E74E-41DF-AAE4-37E8BABFD5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="82">
   <si>
     <t>;</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Central HPWH Compressors look-up table</t>
   </si>
   <si>
-    <t>8/31/20 - SAC</t>
-  </si>
-  <si>
     <t>8/31/20 - SAC - created initial table from existing ruleset data and compressor capacity (kW) data from Ben Larson</t>
   </si>
   <si>
@@ -273,6 +270,15 @@
   </si>
   <si>
     <t>OutputCap - output heating capacity @ ambient 40 deg F</t>
+  </si>
+  <si>
+    <t>generic</t>
+  </si>
+  <si>
+    <t>6/22/21 - SAC - added 'generic' 5, 11, 20, 26, 40 &amp; 45 kW compressor types</t>
+  </si>
+  <si>
+    <t>6/22/21 - SAC</t>
   </si>
 </sst>
 </file>
@@ -447,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -490,6 +496,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD161AC-8F54-43FE-9249-2CA51C7B791C}">
-  <dimension ref="A1:K71"/>
+  <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +855,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -864,7 +871,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -880,13 +887,16 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -901,7 +911,7 @@
         <v>5</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="7"/>
@@ -914,16 +924,16 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="12" t="s">
-        <v>33</v>
-      </c>
       <c r="K11" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -935,7 +945,7 @@
         <v>48</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K12" s="10">
         <v>10</v>
@@ -953,7 +963,7 @@
         <v>49</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K13" s="10">
         <v>21</v>
@@ -967,13 +977,13 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I14" s="9">
         <v>50</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K14" s="10">
         <v>29</v>
@@ -988,7 +998,7 @@
         <v>45</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K15" s="10">
         <v>41</v>
@@ -1004,7 +1014,7 @@
         <v>51</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K16" s="10">
         <v>49</v>
@@ -1012,14 +1022,14 @@
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="2"/>
       <c r="I17" s="9">
         <v>52</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K17" s="10">
         <v>57</v>
@@ -1027,23 +1037,23 @@
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="I18" s="9">
         <v>53</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K18" s="10">
         <v>5</v>
@@ -1061,7 +1071,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19" t="str">
         <f xml:space="preserve"> F19 &amp; "  (" &amp; D19 &amp; "kW cap @ 40F)"</f>
@@ -1071,7 +1081,7 @@
         <v>54</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K19" s="10">
         <v>11</v>
@@ -1082,24 +1092,24 @@
         <v>49</v>
       </c>
       <c r="D20" s="9">
-        <f t="shared" ref="D20:D69" si="0">VLOOKUP( MOD(C20,100), $I$12:$K$38, 3, FALSE )</f>
+        <f t="shared" ref="D20:D75" si="0">VLOOKUP( MOD(C20,100), $I$12:$K$38, 3, FALSE )</f>
         <v>21</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G20" t="str">
-        <f t="shared" ref="G20:G69" si="1" xml:space="preserve"> F20 &amp; "  (" &amp; D20 &amp; "kW cap @ 40F)"</f>
+        <f t="shared" ref="G20:G75" si="1" xml:space="preserve"> F20 &amp; "  (" &amp; D20 &amp; "kW cap @ 40F)"</f>
         <v>Colmac CxA-10  (21kW cap @ 40F)</v>
       </c>
       <c r="I20" s="9">
         <v>55</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K20" s="10">
         <v>20</v>
@@ -1117,7 +1127,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="1"/>
@@ -1127,7 +1137,7 @@
         <v>56</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K21" s="10">
         <v>26</v>
@@ -1145,7 +1155,7 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
@@ -1155,7 +1165,7 @@
         <v>46</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K22" s="10">
         <v>40</v>
@@ -1173,7 +1183,7 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
@@ -1183,7 +1193,7 @@
         <v>47</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K23" s="10">
         <v>45</v>
@@ -1201,7 +1211,7 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
@@ -1211,7 +1221,7 @@
         <v>67</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K24" s="10">
         <v>11</v>
@@ -1229,7 +1239,7 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
@@ -1239,7 +1249,7 @@
         <v>68</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K25" s="10">
         <v>20</v>
@@ -1257,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="1"/>
@@ -1267,7 +1277,7 @@
         <v>69</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K26" s="10">
         <v>26</v>
@@ -1285,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="1"/>
@@ -1295,7 +1305,7 @@
         <v>70</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K27" s="10">
         <v>40</v>
@@ -1313,7 +1323,7 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="1"/>
@@ -1323,7 +1333,7 @@
         <v>71</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K28" s="10">
         <v>45</v>
@@ -1341,7 +1351,7 @@
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
@@ -1351,7 +1361,7 @@
         <v>57</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K29" s="10">
         <v>4</v>
@@ -1369,15 +1379,22 @@
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C250A  (45kW cap @ 40F)</v>
       </c>
-      <c r="I30" s="9"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="10"/>
+      <c r="I30" s="9">
+        <v>91</v>
+      </c>
+      <c r="J30" s="20" t="str">
+        <f>"Generic-" &amp; K30</f>
+        <v>Generic-5</v>
+      </c>
+      <c r="K30" s="10">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
@@ -1391,15 +1408,22 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C60A-C  (11kW cap @ 40F)</v>
       </c>
-      <c r="I31" s="9"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="10"/>
+      <c r="I31" s="9">
+        <v>92</v>
+      </c>
+      <c r="J31" s="20" t="str">
+        <f t="shared" ref="J31:J35" si="2">"Generic-" &amp; K31</f>
+        <v>Generic-11</v>
+      </c>
+      <c r="K31" s="10">
+        <v>11</v>
+      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
@@ -1413,15 +1437,22 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C90A-C  (20kW cap @ 40F)</v>
       </c>
-      <c r="I32" s="9"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="10"/>
+      <c r="I32" s="9">
+        <v>93</v>
+      </c>
+      <c r="J32" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Generic-20</v>
+      </c>
+      <c r="K32" s="10">
+        <v>20</v>
+      </c>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
@@ -1435,15 +1466,22 @@
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C125A-C  (26kW cap @ 40F)</v>
       </c>
-      <c r="I33" s="9"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="10"/>
+      <c r="I33" s="9">
+        <v>94</v>
+      </c>
+      <c r="J33" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Generic-26</v>
+      </c>
+      <c r="K33" s="10">
+        <v>26</v>
+      </c>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
@@ -1457,15 +1495,22 @@
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C185A-C  (40kW cap @ 40F)</v>
       </c>
-      <c r="I34" s="9"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="10"/>
+      <c r="I34" s="9">
+        <v>95</v>
+      </c>
+      <c r="J34" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Generic-40</v>
+      </c>
+      <c r="K34" s="10">
+        <v>40</v>
+      </c>
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
@@ -1479,15 +1524,22 @@
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C250A-C  (45kW cap @ 40F)</v>
       </c>
-      <c r="I35" s="9"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="10"/>
+      <c r="I35" s="9">
+        <v>96</v>
+      </c>
+      <c r="J35" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Generic-45</v>
+      </c>
+      <c r="K35" s="10">
+        <v>45</v>
+      </c>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
@@ -1501,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="1"/>
@@ -1523,7 +1575,7 @@
         <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="1"/>
@@ -1545,7 +1597,7 @@
         <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="1"/>
@@ -1567,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="1"/>
@@ -1586,7 +1638,7 @@
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="1"/>
@@ -1605,7 +1657,7 @@
         <v>0</v>
       </c>
       <c r="F41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="1"/>
@@ -1624,7 +1676,7 @@
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="1"/>
@@ -1643,7 +1695,7 @@
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="1"/>
@@ -1662,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="1"/>
@@ -1681,7 +1733,7 @@
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="1"/>
@@ -1700,7 +1752,7 @@
         <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="1"/>
@@ -1719,7 +1771,7 @@
         <v>0</v>
       </c>
       <c r="F47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="1"/>
@@ -1738,7 +1790,7 @@
         <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="1"/>
@@ -1757,7 +1809,7 @@
         <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="1"/>
@@ -1776,7 +1828,7 @@
         <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="1"/>
@@ -1795,7 +1847,7 @@
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="1"/>
@@ -1814,7 +1866,7 @@
         <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="1"/>
@@ -1833,7 +1885,7 @@
         <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="1"/>
@@ -1852,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="1"/>
@@ -1871,7 +1923,7 @@
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="1"/>
@@ -1890,7 +1942,7 @@
         <v>0</v>
       </c>
       <c r="F56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="1"/>
@@ -1909,7 +1961,7 @@
         <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="1"/>
@@ -1928,7 +1980,7 @@
         <v>0</v>
       </c>
       <c r="F58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="1"/>
@@ -1947,7 +1999,7 @@
         <v>0</v>
       </c>
       <c r="F59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G59" t="str">
         <f t="shared" si="1"/>
@@ -1966,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="1"/>
@@ -1985,7 +2037,7 @@
         <v>0</v>
       </c>
       <c r="F61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="1"/>
@@ -2004,7 +2056,7 @@
         <v>0</v>
       </c>
       <c r="F62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="1"/>
@@ -2023,7 +2075,7 @@
         <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="1"/>
@@ -2042,7 +2094,7 @@
         <v>0</v>
       </c>
       <c r="F64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="1"/>
@@ -2061,7 +2113,7 @@
         <v>0</v>
       </c>
       <c r="F65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="1"/>
@@ -2080,7 +2132,7 @@
         <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" si="1"/>
@@ -2099,7 +2151,7 @@
         <v>0</v>
       </c>
       <c r="F67" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G67" t="str">
         <f t="shared" si="1"/>
@@ -2118,7 +2170,7 @@
         <v>0</v>
       </c>
       <c r="F68" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" si="1"/>
@@ -2137,7 +2189,7 @@
         <v>0</v>
       </c>
       <c r="F69" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="1"/>
@@ -2145,22 +2197,136 @@
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="18" t="s">
+      <c r="C70" s="1">
+        <v>991</v>
+      </c>
+      <c r="D70" s="9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E70" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F70" t="s">
+        <v>79</v>
+      </c>
+      <c r="G70" t="str">
+        <f t="shared" si="1"/>
+        <v>generic  (5kW cap @ 40F)</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C71" s="1">
+        <v>992</v>
+      </c>
+      <c r="D71" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E71" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F71" t="s">
+        <v>79</v>
+      </c>
+      <c r="G71" t="str">
+        <f t="shared" si="1"/>
+        <v>generic  (11kW cap @ 40F)</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C72" s="1">
+        <v>993</v>
+      </c>
+      <c r="D72" s="9">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E72" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F72" t="s">
+        <v>79</v>
+      </c>
+      <c r="G72" t="str">
+        <f t="shared" si="1"/>
+        <v>generic  (20kW cap @ 40F)</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C73" s="1">
+        <v>994</v>
+      </c>
+      <c r="D73" s="9">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="E73" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F73" t="s">
+        <v>79</v>
+      </c>
+      <c r="G73" t="str">
+        <f t="shared" si="1"/>
+        <v>generic  (26kW cap @ 40F)</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C74" s="1">
+        <v>995</v>
+      </c>
+      <c r="D74" s="9">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E74" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F74" t="s">
+        <v>79</v>
+      </c>
+      <c r="G74" t="str">
+        <f t="shared" si="1"/>
+        <v>generic  (40kW cap @ 40F)</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C75" s="1">
+        <v>996</v>
+      </c>
+      <c r="D75" s="9">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="E75" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>79</v>
+      </c>
+      <c r="G75" t="str">
+        <f t="shared" si="1"/>
+        <v>generic  (45kW cap @ 40F)</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C76" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D76" s="19">
+        <v>0</v>
+      </c>
+      <c r="E76" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F76" t="s">
         <v>75</v>
       </c>
-      <c r="D70" s="19">
-        <v>0</v>
-      </c>
-      <c r="E70" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F70" t="s">
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SVN Revision #6936 by scriswellwsf       CBECC-22 (1226) executables and ruleset mods enabling new simulation to facilitate load passing from CSE into E+
</commit_message>
<xml_diff>
--- a/Documentation/T24N/T24R_CentralHPWHCompressors.xlsx
+++ b/Documentation/T24N/T24R_CentralHPWHCompressors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\svn-CEC\SF_CBECC-Res\trunk\RulesetDev\Rulesets\CA Res\Rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Com\branches\CBECC-Com_MFamRestructure\RulesetDev\Rulesets\shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237A9B4C-7BB9-46CA-B308-5073F6A644BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B69B54-5AAE-4277-BC0A-93E5A1B27026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="1575" windowWidth="24210" windowHeight="12930" xr2:uid="{06DD2E85-E74E-41DF-AAE4-37E8BABFD5C8}"/>
+    <workbookView xWindow="2430" yWindow="1140" windowWidth="25470" windowHeight="13905" xr2:uid="{06DD2E85-E74E-41DF-AAE4-37E8BABFD5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="104">
   <si>
     <t>;</t>
   </si>
@@ -278,7 +278,73 @@
     <t>6/22/21 - SAC - added 'generic' 5, 11, 20, 26, 40 &amp; 45 kW compressor types</t>
   </si>
   <si>
-    <t>6/22/21 - SAC</t>
+    <t>Colmac CxA-10 (MP)</t>
+  </si>
+  <si>
+    <t>Colmac CxA-15 (MP)</t>
+  </si>
+  <si>
+    <t>Colmac CxA-20 (MP)</t>
+  </si>
+  <si>
+    <t>Colmac CxA-25 (MP)</t>
+  </si>
+  <si>
+    <t>Colmac CxA-30 (MP)</t>
+  </si>
+  <si>
+    <t>Colmac CxV-5 (MP)</t>
+  </si>
+  <si>
+    <t>Rheem HPHD-135VNU (vertical MP)</t>
+  </si>
+  <si>
+    <t>Rheem HPHD-60HNU (horiz MP)</t>
+  </si>
+  <si>
+    <t>Rheem HPHD-60VNU (vertical MP)</t>
+  </si>
+  <si>
+    <t>Rheem HPHD-135HNU (horiz MP)</t>
+  </si>
+  <si>
+    <t>multi pass additions - SAC 01/18/22</t>
+  </si>
+  <si>
+    <t>Colmac CxA-10 (MP, 21kW cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Colmac CxA-15 (MP, 29kW cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Colmac CxA-20 (MP, 41kW cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Colmac CxA-25 (MP, 50kW cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Colmac CxA-30 (MP, 58kW cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Rheem HPHD-135VNU (vertical MP, 30kW cap @ 45F)</t>
+  </si>
+  <si>
+    <t>Colmac CxV-5 (MP, 14kW cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Rheem HPHD-135HNU (horiz MP, 30kW cap @ 45F)</t>
+  </si>
+  <si>
+    <t>Rheem HPHD-60HNU (horiz MP, 12kW cap @ 45F)</t>
+  </si>
+  <si>
+    <t>Rheem HPHD-60VNU (vertical MP, 12kW cap @ 45F)</t>
+  </si>
+  <si>
+    <t>01/18/22 - SAC - added multi pass compressor types</t>
+  </si>
+  <si>
+    <t>01/18/22 - SAC</t>
   </si>
 </sst>
 </file>
@@ -330,7 +396,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -449,11 +515,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -497,6 +572,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -811,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD161AC-8F54-43FE-9249-2CA51C7B791C}">
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:K88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +901,7 @@
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="2.85546875" customWidth="1"/>
     <col min="6" max="6" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.5703125" customWidth="1"/>
     <col min="8" max="8" width="4.28515625" customWidth="1"/>
     <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -855,7 +931,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -887,7 +963,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -895,113 +971,106 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>77</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>12</v>
-      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="I12" s="9">
-        <v>48</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="10">
-        <v>10</v>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
       <c r="C13" s="1"/>
       <c r="I13" s="9">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K13" s="10">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>78</v>
-      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1"/>
       <c r="I14" s="9">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K14" s="10">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>78</v>
+      </c>
       <c r="I15" s="9">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K15" s="10">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1009,577 +1078,570 @@
         <v>0</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
       <c r="I16" s="9">
+        <v>45</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="10">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="I17" s="9">
         <v>51</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K17" s="10">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="I17" s="9">
+      <c r="D18" s="2"/>
+      <c r="I18" s="9">
         <v>52</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K18" s="10">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="3" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="3" t="s">
+      <c r="E19" s="5"/>
+      <c r="F19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I19" s="9">
         <v>53</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K19" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="1">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="1">
         <v>48</v>
       </c>
-      <c r="D19" s="16">
-        <f>VLOOKUP( MOD(C19,100), $I$12:$K$38, 3, FALSE )</f>
+      <c r="D20" s="16">
+        <f>VLOOKUP( MOD(C20,100), $I$13:$K$39, 3, FALSE )</f>
         <v>10</v>
       </c>
-      <c r="E19" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="E20" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
         <v>13</v>
       </c>
-      <c r="G19" t="str">
-        <f xml:space="preserve"> F19 &amp; "  (" &amp; D19 &amp; "kW cap @ 40F)"</f>
+      <c r="G20" t="str">
+        <f xml:space="preserve"> F20 &amp; "  (" &amp; D20 &amp; "kW cap @ 40F)"</f>
         <v>Colmac CxV-5  (10kW cap @ 40F)</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I20" s="9">
         <v>54</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K20" s="10">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="1">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="1">
         <v>49</v>
       </c>
-      <c r="D20" s="9">
-        <f t="shared" ref="D20:D75" si="0">VLOOKUP( MOD(C20,100), $I$12:$K$38, 3, FALSE )</f>
+      <c r="D21" s="9">
+        <f t="shared" ref="D21:D86" si="0">VLOOKUP( MOD(C21,100), $I$13:$K$39, 3, FALSE )</f>
         <v>21</v>
       </c>
-      <c r="E20" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="E21" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
         <v>14</v>
       </c>
-      <c r="G20" t="str">
-        <f t="shared" ref="G20:G75" si="1" xml:space="preserve"> F20 &amp; "  (" &amp; D20 &amp; "kW cap @ 40F)"</f>
+      <c r="G21" t="str">
+        <f t="shared" ref="G21:G86" si="1" xml:space="preserve"> F21 &amp; "  (" &amp; D21 &amp; "kW cap @ 40F)"</f>
         <v>Colmac CxA-10  (21kW cap @ 40F)</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I21" s="9">
         <v>55</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K21" s="10">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C21" s="1">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="1">
         <v>50</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D22" s="9">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="E21" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="E22" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
         <v>15</v>
       </c>
-      <c r="G21" t="str">
+      <c r="G22" t="str">
         <f t="shared" si="1"/>
         <v>Colmac CxA-15  (29kW cap @ 40F)</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I22" s="9">
         <v>56</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J22" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K22" s="10">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="1">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="1">
         <v>45</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D23" s="9">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="E22" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="E23" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
         <v>16</v>
       </c>
-      <c r="G22" t="str">
+      <c r="G23" t="str">
         <f t="shared" si="1"/>
         <v>Colmac CxA-20  (41kW cap @ 40F)</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I23" s="9">
         <v>46</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J23" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K23" s="10">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C23" s="1">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="1">
         <v>51</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D24" s="9">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="E23" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="E24" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
         <v>17</v>
       </c>
-      <c r="G23" t="str">
+      <c r="G24" t="str">
         <f t="shared" si="1"/>
         <v>Colmac CxA-25  (49kW cap @ 40F)</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I24" s="9">
         <v>47</v>
       </c>
-      <c r="J23" s="8" t="s">
+      <c r="J24" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K23" s="10">
+      <c r="K24" s="10">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="1">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="1">
         <v>52</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D25" s="9">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="E24" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="E25" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
         <v>18</v>
       </c>
-      <c r="G24" t="str">
+      <c r="G25" t="str">
         <f t="shared" si="1"/>
         <v>Colmac CxA-30  (57kW cap @ 40F)</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I25" s="9">
         <v>67</v>
       </c>
-      <c r="J24" s="8" t="s">
+      <c r="J25" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K25" s="10">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="1">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C26" s="1">
         <v>53</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D26" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E25" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="E26" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
         <v>19</v>
       </c>
-      <c r="G25" t="str">
+      <c r="G26" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C25A  (5kW cap @ 40F)</v>
       </c>
-      <c r="I25" s="9">
+      <c r="I26" s="9">
         <v>68</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="J26" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K26" s="10">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="1">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C27" s="1">
         <v>54</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D27" s="9">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="E26" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="E27" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
         <v>20</v>
       </c>
-      <c r="G26" t="str">
+      <c r="G27" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C60A  (11kW cap @ 40F)</v>
       </c>
-      <c r="I26" s="9">
+      <c r="I27" s="9">
         <v>69</v>
       </c>
-      <c r="J26" s="8" t="s">
+      <c r="J27" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K26" s="10">
+      <c r="K27" s="10">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="1">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C28" s="1">
         <v>55</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D28" s="9">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E27" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="E28" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
         <v>21</v>
       </c>
-      <c r="G27" t="str">
+      <c r="G28" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C90A  (20kW cap @ 40F)</v>
       </c>
-      <c r="I27" s="9">
+      <c r="I28" s="9">
         <v>70</v>
       </c>
-      <c r="J27" s="8" t="s">
+      <c r="J28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="K27" s="10">
+      <c r="K28" s="10">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C28" s="1">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C29" s="1">
         <v>56</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D29" s="9">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="E28" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="E29" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
         <v>22</v>
       </c>
-      <c r="G28" t="str">
+      <c r="G29" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C125A  (26kW cap @ 40F)</v>
       </c>
-      <c r="I28" s="9">
+      <c r="I29" s="9">
         <v>71</v>
       </c>
-      <c r="J28" s="8" t="s">
+      <c r="J29" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K28" s="10">
+      <c r="K29" s="10">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C29" s="1">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C30" s="1">
         <v>46</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D30" s="9">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E29" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="E30" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
         <v>23</v>
       </c>
-      <c r="G29" t="str">
+      <c r="G30" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C185A  (40kW cap @ 40F)</v>
       </c>
-      <c r="I29" s="9">
+      <c r="I30" s="9">
         <v>57</v>
       </c>
-      <c r="J29" s="8" t="s">
+      <c r="J30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="K29" s="10">
+      <c r="K30" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C30" s="1">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C31" s="1">
         <v>47</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D31" s="9">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="E30" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="E31" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
         <v>24</v>
       </c>
-      <c r="G30" t="str">
+      <c r="G31" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C250A  (45kW cap @ 40F)</v>
       </c>
-      <c r="I30" s="9">
+      <c r="I31" s="9">
         <v>91</v>
       </c>
-      <c r="J30" s="20" t="str">
-        <f>"Generic-" &amp; K30</f>
+      <c r="J31" s="20" t="str">
+        <f>"Generic-" &amp; K31</f>
         <v>Generic-5</v>
       </c>
-      <c r="K30" s="10">
+      <c r="K31" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C31" s="1">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C32" s="1">
         <v>67</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D32" s="9">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="E31" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="E32" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
         <v>37</v>
       </c>
-      <c r="G31" t="str">
+      <c r="G32" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C60A-C  (11kW cap @ 40F)</v>
       </c>
-      <c r="I31" s="9">
+      <c r="I32" s="9">
         <v>92</v>
       </c>
-      <c r="J31" s="20" t="str">
-        <f t="shared" ref="J31:J35" si="2">"Generic-" &amp; K31</f>
+      <c r="J32" s="20" t="str">
+        <f t="shared" ref="J32:J36" si="2">"Generic-" &amp; K32</f>
         <v>Generic-11</v>
       </c>
-      <c r="K31" s="10">
+      <c r="K32" s="10">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C32" s="1">
+    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C33" s="1">
         <v>68</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D33" s="9">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E32" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="E33" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
         <v>38</v>
       </c>
-      <c r="G32" t="str">
+      <c r="G33" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C90A-C  (20kW cap @ 40F)</v>
       </c>
-      <c r="I32" s="9">
+      <c r="I33" s="9">
         <v>93</v>
       </c>
-      <c r="J32" s="20" t="str">
+      <c r="J33" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Generic-20</v>
       </c>
-      <c r="K32" s="10">
+      <c r="K33" s="10">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C33" s="1">
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C34" s="1">
         <v>69</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D34" s="9">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="E33" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="E34" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
         <v>34</v>
       </c>
-      <c r="G33" t="str">
+      <c r="G34" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C125A-C  (26kW cap @ 40F)</v>
       </c>
-      <c r="I33" s="9">
+      <c r="I34" s="9">
         <v>94</v>
       </c>
-      <c r="J33" s="20" t="str">
+      <c r="J34" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Generic-26</v>
       </c>
-      <c r="K33" s="10">
+      <c r="K34" s="10">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C34" s="1">
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C35" s="1">
         <v>70</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D35" s="9">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E34" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="E35" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
         <v>35</v>
       </c>
-      <c r="G34" t="str">
+      <c r="G35" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C185A-C  (40kW cap @ 40F)</v>
       </c>
-      <c r="I34" s="9">
+      <c r="I35" s="9">
         <v>95</v>
       </c>
-      <c r="J34" s="20" t="str">
+      <c r="J35" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Generic-40</v>
       </c>
-      <c r="K34" s="10">
+      <c r="K35" s="10">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C35" s="1">
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C36" s="1">
         <v>71</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D36" s="9">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="E35" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="E36" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
         <v>36</v>
       </c>
-      <c r="G35" t="str">
+      <c r="G36" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C250A-C  (45kW cap @ 40F)</v>
       </c>
-      <c r="I35" s="9">
+      <c r="I36" s="9">
         <v>96</v>
       </c>
-      <c r="J35" s="20" t="str">
+      <c r="J36" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Generic-45</v>
       </c>
-      <c r="K35" s="10">
+      <c r="K36" s="10">
         <v>45</v>
       </c>
-    </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C36" s="1">
-        <v>57</v>
-      </c>
-      <c r="D36" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F36" t="s">
-        <v>30</v>
-      </c>
-      <c r="G36" t="str">
-        <f t="shared" si="1"/>
-        <v>Sanden GS3-45HPA-US  (4kW cap @ 40F)</v>
-      </c>
-      <c r="I36" s="9"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="10"/>
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
-        <v>153</v>
+        <v>57</v>
       </c>
       <c r="D37" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E37" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP025-*-***N****  (5kW cap @ 40F)</v>
+        <v>Sanden GS3-45HPA-US  (4kW cap @ 40F)</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="8"/>
@@ -1587,749 +1649,946 @@
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D38" s="9">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E38" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP060-*-***N****  (11kW cap @ 40F)</v>
-      </c>
-      <c r="I38" s="11"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="13"/>
+        <v>Lochinvar AHP025-*-***N****  (5kW cap @ 40F)</v>
+      </c>
+      <c r="I38" s="9"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="10"/>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D39" s="9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E39" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP090-*-***N****  (20kW cap @ 40F)</v>
-      </c>
+        <v>Lochinvar AHP060-*-***N****  (11kW cap @ 40F)</v>
+      </c>
+      <c r="I39" s="11"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="13"/>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D40" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E40" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP125-*-***N****  (26kW cap @ 40F)</v>
+        <v>Lochinvar AHP090-*-***N****  (20kW cap @ 40F)</v>
       </c>
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="D41" s="9">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E41" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP185-*-***N****  (40kW cap @ 40F)</v>
+        <v>Lochinvar AHP125-*-***N****  (26kW cap @ 40F)</v>
       </c>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D42" s="9">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E42" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP250-*-***N****  (45kW cap @ 40F)</v>
+        <v>Lochinvar AHP185-*-***N****  (40kW cap @ 40F)</v>
       </c>
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
-        <v>253</v>
+        <v>147</v>
       </c>
       <c r="D43" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="E43" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-25-*-***N****  (5kW cap @ 40F)</v>
+        <v>Lochinvar AHP250-*-***N****  (45kW cap @ 40F)</v>
       </c>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D44" s="9">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E44" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-60-*-***N****  (11kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-25-*-***N****  (5kW cap @ 40F)</v>
       </c>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D45" s="9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E45" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-90-*-***N****  (20kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-60-*-***N****  (11kW cap @ 40F)</v>
       </c>
     </row>
     <row r="46" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D46" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E46" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-125-*-***N****  (26kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-90-*-***N****  (20kW cap @ 40F)</v>
       </c>
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="D47" s="9">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E47" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-185-*-***N****  (40kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-125-*-***N****  (26kW cap @ 40F)</v>
       </c>
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D48" s="9">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E48" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-250-*-***N****  (45kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-185-*-***N****  (40kW cap @ 40F)</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
-        <v>353</v>
+        <v>247</v>
       </c>
       <c r="D49" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="E49" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-25-*-***N****  (5kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-250-*-***N****  (45kW cap @ 40F)</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D50" s="9">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E50" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-60-*-***N****  (11kW cap @ 40F)</v>
+        <v>State SHPA-25-*-***N****  (5kW cap @ 40F)</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D51" s="9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E51" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-90-*-***N****  (20kW cap @ 40F)</v>
+        <v>State SHPA-60-*-***N****  (11kW cap @ 40F)</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D52" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E52" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-125-*-***N****  (26kW cap @ 40F)</v>
+        <v>State SHPA-90-*-***N****  (20kW cap @ 40F)</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="D53" s="9">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E53" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-185-*-***N****  (40kW cap @ 40F)</v>
+        <v>State SHPA-125-*-***N****  (26kW cap @ 40F)</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D54" s="9">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E54" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-250-*-***N****  (45kW cap @ 40F)</v>
+        <v>State SHPA-185-*-***N****  (40kW cap @ 40F)</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
-        <v>167</v>
+        <v>347</v>
       </c>
       <c r="D55" s="9">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="E55" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP060-*-***C****  (11kW cap @ 40F)</v>
+        <v>State SHPA-250-*-***N****  (45kW cap @ 40F)</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C56" s="1">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D56" s="9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E56" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP090-*-***C****  (20kW cap @ 40F)</v>
+        <v>Lochinvar AHP060-*-***C****  (11kW cap @ 40F)</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C57" s="1">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D57" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E57" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP125-*-***C****  (26kW cap @ 40F)</v>
+        <v>Lochinvar AHP090-*-***C****  (20kW cap @ 40F)</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C58" s="1">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D58" s="9">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E58" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP185-*-***C****  (40kW cap @ 40F)</v>
+        <v>Lochinvar AHP125-*-***C****  (26kW cap @ 40F)</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C59" s="1">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D59" s="9">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E59" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F59" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G59" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP250-*-***C****  (45kW cap @ 40F)</v>
+        <v>Lochinvar AHP185-*-***C****  (40kW cap @ 40F)</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C60" s="1">
-        <v>267</v>
+        <v>171</v>
       </c>
       <c r="D60" s="9">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="E60" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-60-*-***C****  (11kW cap @ 40F)</v>
+        <v>Lochinvar AHP250-*-***C****  (45kW cap @ 40F)</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C61" s="1">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D61" s="9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E61" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F61" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-90-*-***C****  (20kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-60-*-***C****  (11kW cap @ 40F)</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C62" s="1">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D62" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E62" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F62" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-125-*-***C****  (26kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-90-*-***C****  (20kW cap @ 40F)</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C63" s="1">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D63" s="9">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E63" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-185-*-***C****  (40kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-125-*-***C****  (26kW cap @ 40F)</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C64" s="1">
+        <v>270</v>
+      </c>
+      <c r="D64" s="9">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E64" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F64" t="s">
+        <v>49</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="1"/>
+        <v>A. O. Smith AHPA-185-*-***C****  (40kW cap @ 40F)</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C65" s="1">
         <v>271</v>
       </c>
-      <c r="D64" s="9">
+      <c r="D65" s="9">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="E64" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="E65" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F65" t="s">
         <v>50</v>
       </c>
-      <c r="G64" t="str">
+      <c r="G65" t="str">
         <f t="shared" si="1"/>
         <v>A. O. Smith AHPA-250-*-***C****  (45kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="1">
+    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C66" s="1">
         <v>367</v>
       </c>
-      <c r="D65" s="9">
+      <c r="D66" s="9">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="E65" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="E66" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F66" t="s">
         <v>70</v>
       </c>
-      <c r="G65" t="str">
+      <c r="G66" t="str">
         <f t="shared" si="1"/>
         <v>State SHPA-60-*-***C****  (11kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="1">
+    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C67" s="1">
         <v>368</v>
       </c>
-      <c r="D66" s="9">
+      <c r="D67" s="9">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E66" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="E67" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F67" t="s">
         <v>71</v>
       </c>
-      <c r="G66" t="str">
+      <c r="G67" t="str">
         <f t="shared" si="1"/>
         <v>State SHPA-90-*-***C****  (20kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="1">
+    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C68" s="1">
         <v>369</v>
       </c>
-      <c r="D67" s="9">
+      <c r="D68" s="9">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="E67" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="E68" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F68" t="s">
         <v>51</v>
       </c>
-      <c r="G67" t="str">
+      <c r="G68" t="str">
         <f t="shared" si="1"/>
         <v>State SHPA-125-*-***C****  (26kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C68" s="1">
+    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C69" s="1">
         <v>370</v>
       </c>
-      <c r="D68" s="9">
+      <c r="D69" s="9">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E68" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F68" t="s">
+      <c r="E69" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F69" t="s">
         <v>52</v>
       </c>
-      <c r="G68" t="str">
+      <c r="G69" t="str">
         <f t="shared" si="1"/>
         <v>State SHPA-185-*-***C****  (40kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="1">
+    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C70" s="1">
         <v>371</v>
       </c>
-      <c r="D69" s="9">
+      <c r="D70" s="9">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="E69" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="E70" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F70" t="s">
         <v>53</v>
       </c>
-      <c r="G69" t="str">
+      <c r="G70" t="str">
         <f t="shared" si="1"/>
         <v>State SHPA-250-*-***C****  (45kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="1">
+    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C71" s="1">
+        <v>77</v>
+      </c>
+      <c r="D71" s="9">
+        <v>14</v>
+      </c>
+      <c r="E71" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F71" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="G71" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="H71" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C72" s="1">
+        <v>78</v>
+      </c>
+      <c r="D72" s="9">
+        <v>21</v>
+      </c>
+      <c r="E72" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F72" t="s">
+        <v>81</v>
+      </c>
+      <c r="G72" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C73" s="1">
+        <v>79</v>
+      </c>
+      <c r="D73" s="9">
+        <v>29</v>
+      </c>
+      <c r="E73" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F73" t="s">
+        <v>82</v>
+      </c>
+      <c r="G73" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C74" s="1">
+        <v>80</v>
+      </c>
+      <c r="D74" s="9">
+        <v>41</v>
+      </c>
+      <c r="E74" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F74" t="s">
+        <v>83</v>
+      </c>
+      <c r="G74" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="75" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C75" s="1">
+        <v>81</v>
+      </c>
+      <c r="D75" s="9">
+        <v>50</v>
+      </c>
+      <c r="E75" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>84</v>
+      </c>
+      <c r="G75" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C76" s="1">
+        <v>82</v>
+      </c>
+      <c r="D76" s="9">
+        <v>58</v>
+      </c>
+      <c r="E76" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F76" t="s">
+        <v>85</v>
+      </c>
+      <c r="G76" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C77" s="1">
+        <v>83</v>
+      </c>
+      <c r="D77" s="9">
+        <v>12</v>
+      </c>
+      <c r="E77" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F77" t="s">
+        <v>88</v>
+      </c>
+      <c r="G77" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C78" s="1">
+        <v>84</v>
+      </c>
+      <c r="D78" s="9">
+        <v>12</v>
+      </c>
+      <c r="E78" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F78" t="s">
+        <v>89</v>
+      </c>
+      <c r="G78" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="79" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C79" s="1">
+        <v>85</v>
+      </c>
+      <c r="D79" s="9">
+        <v>30</v>
+      </c>
+      <c r="E79" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F79" t="s">
+        <v>90</v>
+      </c>
+      <c r="G79" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C80" s="1">
+        <v>86</v>
+      </c>
+      <c r="D80" s="9">
+        <v>30</v>
+      </c>
+      <c r="E80" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F80" t="s">
+        <v>87</v>
+      </c>
+      <c r="G80" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C81" s="1">
         <v>991</v>
       </c>
-      <c r="D70" s="9">
+      <c r="D81" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E70" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="E81" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F81" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="G70" t="str">
+      <c r="G81" s="21" t="str">
         <f t="shared" si="1"/>
         <v>generic  (5kW cap @ 40F)</v>
       </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C71" s="1">
+      <c r="H81" s="21"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C82" s="1">
         <v>992</v>
       </c>
-      <c r="D71" s="9">
+      <c r="D82" s="9">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="E71" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="E82" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F82" t="s">
         <v>79</v>
       </c>
-      <c r="G71" t="str">
+      <c r="G82" t="str">
         <f t="shared" si="1"/>
         <v>generic  (11kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="1">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C83" s="1">
         <v>993</v>
       </c>
-      <c r="D72" s="9">
+      <c r="D83" s="9">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E72" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F72" t="s">
+      <c r="E83" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F83" t="s">
         <v>79</v>
       </c>
-      <c r="G72" t="str">
+      <c r="G83" t="str">
         <f t="shared" si="1"/>
         <v>generic  (20kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="1">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C84" s="1">
         <v>994</v>
       </c>
-      <c r="D73" s="9">
+      <c r="D84" s="9">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="E73" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F73" t="s">
+      <c r="E84" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F84" t="s">
         <v>79</v>
       </c>
-      <c r="G73" t="str">
+      <c r="G84" t="str">
         <f t="shared" si="1"/>
         <v>generic  (26kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="1">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C85" s="1">
         <v>995</v>
       </c>
-      <c r="D74" s="9">
+      <c r="D85" s="9">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E74" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F74" t="s">
+      <c r="E85" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F85" t="s">
         <v>79</v>
       </c>
-      <c r="G74" t="str">
+      <c r="G85" t="str">
         <f t="shared" si="1"/>
         <v>generic  (40kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C75" s="1">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C86" s="1">
         <v>996</v>
       </c>
-      <c r="D75" s="9">
+      <c r="D86" s="9">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="E75" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F75" t="s">
+      <c r="E86" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F86" t="s">
         <v>79</v>
       </c>
-      <c r="G75" t="str">
+      <c r="G86" t="str">
         <f t="shared" si="1"/>
         <v>generic  (45kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="18" t="s">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C87" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D76" s="19">
-        <v>0</v>
-      </c>
-      <c r="E76" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F76" t="s">
+      <c r="D87" s="19">
+        <v>0</v>
+      </c>
+      <c r="E87" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F87" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SVN Revision #6957 by scriswellwsf       CBECC-22 (1227) executables and ruleset source removing ResGarage (and other minor changes)
</commit_message>
<xml_diff>
--- a/Documentation/T24N/T24R_CentralHPWHCompressors.xlsx
+++ b/Documentation/T24N/T24R_CentralHPWHCompressors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Com\branches\CBECC-Com_MFamRestructure\RulesetDev\Rulesets\shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Com\branches\CBECC-Com_MFamRestructure\Documentation\T24N\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B69B54-5AAE-4277-BC0A-93E5A1B27026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19B5DED-5603-40B8-8218-A38C307FE38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2430" yWindow="1140" windowWidth="25470" windowHeight="13905" xr2:uid="{06DD2E85-E74E-41DF-AAE4-37E8BABFD5C8}"/>
+    <workbookView xWindow="29190" yWindow="390" windowWidth="28155" windowHeight="12885" xr2:uid="{06DD2E85-E74E-41DF-AAE4-37E8BABFD5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Scott Criswell</author>
+  </authors>
+  <commentList>
+    <comment ref="K14" authorId="0" shapeId="0" xr:uid="{6303DEEF-C866-46FF-8A24-CA09C6A7EC95}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>SAC 2/3/22:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+updated OutputCap from 10 to 14 per guidance from PK</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="105">
   <si>
     <t>;</t>
   </si>
@@ -344,14 +378,17 @@
     <t>01/18/22 - SAC - added multi pass compressor types</t>
   </si>
   <si>
-    <t>01/18/22 - SAC</t>
+    <t>02/03/22 - SAC</t>
+  </si>
+  <si>
+    <t>02/03/22 - SAC - updated Colmac CxV-5 compressor OutputCap from 10 to 14 kW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,8 +418,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -392,6 +442,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -528,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -559,9 +615,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -573,6 +626,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -886,11 +945,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD161AC-8F54-43FE-9249-2CA51C7B791C}">
-  <dimension ref="A1:K88"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD161AC-8F54-43FE-9249-2CA51C7B791C}">
+  <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +1022,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -971,7 +1030,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -979,113 +1038,106 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>77</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>12</v>
-      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="6"/>
+      <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="I13" s="9">
-        <v>48</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="10">
-        <v>10</v>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
       <c r="C14" s="1"/>
       <c r="I14" s="9">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="21">
         <v>14</v>
-      </c>
-      <c r="K14" s="10">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>78</v>
-      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1"/>
       <c r="I15" s="9">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K15" s="10">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>78</v>
+      </c>
       <c r="I16" s="9">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K16" s="10">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1093,577 +1145,570 @@
         <v>0</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
       <c r="I17" s="9">
+        <v>45</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="10">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="I18" s="9">
         <v>51</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K18" s="10">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="I18" s="9">
+      <c r="D19" s="2"/>
+      <c r="I19" s="9">
         <v>52</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J19" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K19" s="10">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="3" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="3" t="s">
+      <c r="E20" s="5"/>
+      <c r="F20" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I20" s="9">
         <v>53</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K20" s="10">
         <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="1">
-        <v>48</v>
-      </c>
-      <c r="D20" s="16">
-        <f>VLOOKUP( MOD(C20,100), $I$13:$K$39, 3, FALSE )</f>
-        <v>10</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" t="str">
-        <f xml:space="preserve"> F20 &amp; "  (" &amp; D20 &amp; "kW cap @ 40F)"</f>
-        <v>Colmac CxV-5  (10kW cap @ 40F)</v>
-      </c>
-      <c r="I20" s="9">
-        <v>54</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" s="10">
-        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
-        <v>49</v>
-      </c>
-      <c r="D21" s="9">
-        <f t="shared" ref="D21:D86" si="0">VLOOKUP( MOD(C21,100), $I$13:$K$39, 3, FALSE )</f>
-        <v>21</v>
-      </c>
-      <c r="E21" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="22">
+        <f t="shared" ref="D21:D87" si="0">VLOOKUP( MOD(C21,100), $I$14:$K$40, 3, FALSE )</f>
+        <v>14</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" ref="G21:G86" si="1" xml:space="preserve"> F21 &amp; "  (" &amp; D21 &amp; "kW cap @ 40F)"</f>
-        <v>Colmac CxA-10  (21kW cap @ 40F)</v>
+        <f xml:space="preserve"> F21 &amp; "  (" &amp; D21 &amp; "kW cap @ 40F)"</f>
+        <v>Colmac CxV-5  (14kW cap @ 40F)</v>
       </c>
       <c r="I21" s="9">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K21" s="10">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" s="9">
         <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="E22" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="1"/>
-        <v>Colmac CxA-15  (29kW cap @ 40F)</v>
+        <f t="shared" ref="G22:G87" si="1" xml:space="preserve"> F22 &amp; "  (" &amp; D22 &amp; "kW cap @ 40F)"</f>
+        <v>Colmac CxA-10  (21kW cap @ 40F)</v>
       </c>
       <c r="I22" s="9">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K22" s="10">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D23" s="9">
         <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="E23" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
-        <v>Colmac CxA-20  (41kW cap @ 40F)</v>
+        <v>Colmac CxA-15  (29kW cap @ 40F)</v>
       </c>
       <c r="I23" s="9">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K23" s="10">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D24" s="9">
         <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="E24" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
-        <v>Colmac CxA-25  (49kW cap @ 40F)</v>
+        <v>Colmac CxA-20  (41kW cap @ 40F)</v>
       </c>
       <c r="I24" s="9">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K24" s="10">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" s="9">
         <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="E25" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
-        <v>Colmac CxA-30  (57kW cap @ 40F)</v>
+        <v>Colmac CxA-25  (49kW cap @ 40F)</v>
       </c>
       <c r="I25" s="9">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K25" s="10">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E26" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="1"/>
-        <v>Nyle C25A  (5kW cap @ 40F)</v>
+        <v>Colmac CxA-30  (57kW cap @ 40F)</v>
       </c>
       <c r="I26" s="9">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K26" s="10">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27" s="9">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E27" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="1"/>
+        <v>Nyle C25A  (5kW cap @ 40F)</v>
+      </c>
+      <c r="I27" s="9">
+        <v>68</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K27" s="10">
         <v>20</v>
-      </c>
-      <c r="G27" t="str">
-        <f t="shared" si="1"/>
-        <v>Nyle C60A  (11kW cap @ 40F)</v>
-      </c>
-      <c r="I27" s="9">
-        <v>69</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K27" s="10">
-        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" s="9">
         <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F28" t="s">
-        <v>21</v>
-      </c>
       <c r="G28" t="str">
         <f t="shared" si="1"/>
-        <v>Nyle C90A  (20kW cap @ 40F)</v>
+        <v>Nyle C60A  (11kW cap @ 40F)</v>
       </c>
       <c r="I28" s="9">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K28" s="10">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="E29" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
-        <v>Nyle C125A  (26kW cap @ 40F)</v>
+        <v>Nyle C90A  (20kW cap @ 40F)</v>
       </c>
       <c r="I29" s="9">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K29" s="10">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D30" s="9">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="E30" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
-        <v>Nyle C185A  (40kW cap @ 40F)</v>
+        <v>Nyle C125A  (26kW cap @ 40F)</v>
       </c>
       <c r="I30" s="9">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K30" s="10">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D31" s="9">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="E31" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
-        <v>Nyle C250A  (45kW cap @ 40F)</v>
+        <v>Nyle C185A  (40kW cap @ 40F)</v>
       </c>
       <c r="I31" s="9">
-        <v>91</v>
-      </c>
-      <c r="J31" s="20" t="str">
-        <f>"Generic-" &amp; K31</f>
-        <v>Generic-5</v>
+        <v>57</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="K31" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="D32" s="9">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E32" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="1"/>
-        <v>Nyle C60A-C  (11kW cap @ 40F)</v>
+        <v>Nyle C250A  (45kW cap @ 40F)</v>
       </c>
       <c r="I32" s="9">
-        <v>92</v>
-      </c>
-      <c r="J32" s="20" t="str">
-        <f t="shared" ref="J32:J36" si="2">"Generic-" &amp; K32</f>
-        <v>Generic-11</v>
+        <v>91</v>
+      </c>
+      <c r="J32" s="19" t="str">
+        <f>"Generic-" &amp; K32</f>
+        <v>Generic-5</v>
       </c>
       <c r="K32" s="10">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
+        <v>67</v>
+      </c>
+      <c r="D33" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="1"/>
+        <v>Nyle C60A-C  (11kW cap @ 40F)</v>
+      </c>
+      <c r="I33" s="9">
+        <v>92</v>
+      </c>
+      <c r="J33" s="19" t="str">
+        <f t="shared" ref="J33:J37" si="2">"Generic-" &amp; K33</f>
+        <v>Generic-11</v>
+      </c>
+      <c r="K33" s="10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C34" s="1">
         <v>68</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D34" s="9">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E33" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="E34" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
         <v>38</v>
       </c>
-      <c r="G33" t="str">
+      <c r="G34" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C90A-C  (20kW cap @ 40F)</v>
       </c>
-      <c r="I33" s="9">
+      <c r="I34" s="9">
         <v>93</v>
       </c>
-      <c r="J33" s="20" t="str">
+      <c r="J34" s="19" t="str">
         <f t="shared" si="2"/>
         <v>Generic-20</v>
       </c>
-      <c r="K33" s="10">
+      <c r="K34" s="10">
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C34" s="1">
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C35" s="1">
         <v>69</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D35" s="9">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="E34" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="E35" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
         <v>34</v>
       </c>
-      <c r="G34" t="str">
+      <c r="G35" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C125A-C  (26kW cap @ 40F)</v>
       </c>
-      <c r="I34" s="9">
+      <c r="I35" s="9">
         <v>94</v>
       </c>
-      <c r="J34" s="20" t="str">
+      <c r="J35" s="19" t="str">
         <f t="shared" si="2"/>
         <v>Generic-26</v>
       </c>
-      <c r="K34" s="10">
+      <c r="K35" s="10">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C35" s="1">
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C36" s="1">
         <v>70</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D36" s="9">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E35" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="E36" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
         <v>35</v>
       </c>
-      <c r="G35" t="str">
+      <c r="G36" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C185A-C  (40kW cap @ 40F)</v>
       </c>
-      <c r="I35" s="9">
+      <c r="I36" s="9">
         <v>95</v>
       </c>
-      <c r="J35" s="20" t="str">
+      <c r="J36" s="19" t="str">
         <f t="shared" si="2"/>
         <v>Generic-40</v>
       </c>
-      <c r="K35" s="10">
+      <c r="K36" s="10">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C36" s="1">
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C37" s="1">
         <v>71</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D37" s="9">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="E36" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="E37" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" t="s">
         <v>36</v>
       </c>
-      <c r="G36" t="str">
+      <c r="G37" t="str">
         <f t="shared" si="1"/>
         <v>Nyle C250A-C  (45kW cap @ 40F)</v>
       </c>
-      <c r="I36" s="9">
+      <c r="I37" s="9">
         <v>96</v>
       </c>
-      <c r="J36" s="20" t="str">
+      <c r="J37" s="19" t="str">
         <f t="shared" si="2"/>
         <v>Generic-45</v>
       </c>
-      <c r="K36" s="10">
+      <c r="K37" s="10">
         <v>45</v>
       </c>
-    </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C37" s="1">
-        <v>57</v>
-      </c>
-      <c r="D37" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F37" t="s">
-        <v>30</v>
-      </c>
-      <c r="G37" t="str">
-        <f t="shared" si="1"/>
-        <v>Sanden GS3-45HPA-US  (4kW cap @ 40F)</v>
-      </c>
-      <c r="I37" s="9"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="10"/>
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
-        <v>153</v>
+        <v>57</v>
       </c>
       <c r="D38" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E38" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP025-*-***N****  (5kW cap @ 40F)</v>
+        <v>Sanden GS3-45HPA-US  (4kW cap @ 40F)</v>
       </c>
       <c r="I38" s="9"/>
       <c r="J38" s="8"/>
@@ -1671,836 +1716,839 @@
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D39" s="9">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E39" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP060-*-***N****  (11kW cap @ 40F)</v>
-      </c>
-      <c r="I39" s="11"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="13"/>
+        <v>Lochinvar AHP025-*-***N****  (5kW cap @ 40F)</v>
+      </c>
+      <c r="I39" s="9"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="10"/>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D40" s="9">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="E40" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP090-*-***N****  (20kW cap @ 40F)</v>
-      </c>
+        <v>Lochinvar AHP060-*-***N****  (11kW cap @ 40F)</v>
+      </c>
+      <c r="I40" s="11"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="13"/>
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D41" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="E41" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP125-*-***N****  (26kW cap @ 40F)</v>
+        <v>Lochinvar AHP090-*-***N****  (20kW cap @ 40F)</v>
       </c>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="D42" s="9">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="E42" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP185-*-***N****  (40kW cap @ 40F)</v>
+        <v>Lochinvar AHP125-*-***N****  (26kW cap @ 40F)</v>
       </c>
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D43" s="9">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="E43" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP250-*-***N****  (45kW cap @ 40F)</v>
+        <v>Lochinvar AHP185-*-***N****  (40kW cap @ 40F)</v>
       </c>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
-        <v>253</v>
+        <v>147</v>
       </c>
       <c r="D44" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E44" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-25-*-***N****  (5kW cap @ 40F)</v>
+        <v>Lochinvar AHP250-*-***N****  (45kW cap @ 40F)</v>
       </c>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D45" s="9">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E45" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-60-*-***N****  (11kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-25-*-***N****  (5kW cap @ 40F)</v>
       </c>
     </row>
     <row r="46" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D46" s="9">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="E46" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-90-*-***N****  (20kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-60-*-***N****  (11kW cap @ 40F)</v>
       </c>
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D47" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="E47" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F47" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-125-*-***N****  (26kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-90-*-***N****  (20kW cap @ 40F)</v>
       </c>
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="D48" s="9">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="E48" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-185-*-***N****  (40kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-125-*-***N****  (26kW cap @ 40F)</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D49" s="9">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="E49" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-250-*-***N****  (45kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-185-*-***N****  (40kW cap @ 40F)</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
-        <v>353</v>
+        <v>247</v>
       </c>
       <c r="D50" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E50" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-25-*-***N****  (5kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-250-*-***N****  (45kW cap @ 40F)</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D51" s="9">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E51" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-60-*-***N****  (11kW cap @ 40F)</v>
+        <v>State SHPA-25-*-***N****  (5kW cap @ 40F)</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D52" s="9">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="E52" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-90-*-***N****  (20kW cap @ 40F)</v>
+        <v>State SHPA-60-*-***N****  (11kW cap @ 40F)</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D53" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="E53" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-125-*-***N****  (26kW cap @ 40F)</v>
+        <v>State SHPA-90-*-***N****  (20kW cap @ 40F)</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="D54" s="9">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="E54" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-185-*-***N****  (40kW cap @ 40F)</v>
+        <v>State SHPA-125-*-***N****  (26kW cap @ 40F)</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D55" s="9">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="E55" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E55" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-250-*-***N****  (45kW cap @ 40F)</v>
+        <v>State SHPA-185-*-***N****  (40kW cap @ 40F)</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C56" s="1">
-        <v>167</v>
+        <v>347</v>
       </c>
       <c r="D56" s="9">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E56" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E56" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP060-*-***C****  (11kW cap @ 40F)</v>
+        <v>State SHPA-250-*-***N****  (45kW cap @ 40F)</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C57" s="1">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D57" s="9">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="E57" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP090-*-***C****  (20kW cap @ 40F)</v>
+        <v>Lochinvar AHP060-*-***C****  (11kW cap @ 40F)</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C58" s="1">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D58" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="E58" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E58" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F58" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP125-*-***C****  (26kW cap @ 40F)</v>
+        <v>Lochinvar AHP090-*-***C****  (20kW cap @ 40F)</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C59" s="1">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D59" s="9">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="E59" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E59" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F59" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G59" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP185-*-***C****  (40kW cap @ 40F)</v>
+        <v>Lochinvar AHP125-*-***C****  (26kW cap @ 40F)</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C60" s="1">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D60" s="9">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="E60" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E60" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="1"/>
-        <v>Lochinvar AHP250-*-***C****  (45kW cap @ 40F)</v>
+        <v>Lochinvar AHP185-*-***C****  (40kW cap @ 40F)</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C61" s="1">
-        <v>267</v>
+        <v>171</v>
       </c>
       <c r="D61" s="9">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E61" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E61" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F61" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-60-*-***C****  (11kW cap @ 40F)</v>
+        <v>Lochinvar AHP250-*-***C****  (45kW cap @ 40F)</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C62" s="1">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D62" s="9">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="E62" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-90-*-***C****  (20kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-60-*-***C****  (11kW cap @ 40F)</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C63" s="1">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D63" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="E63" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E63" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-125-*-***C****  (26kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-90-*-***C****  (20kW cap @ 40F)</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C64" s="1">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D64" s="9">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="E64" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E64" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F64" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-185-*-***C****  (40kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-125-*-***C****  (26kW cap @ 40F)</v>
       </c>
     </row>
     <row r="65" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C65" s="1">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D65" s="9">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="E65" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E65" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-250-*-***C****  (45kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-185-*-***C****  (40kW cap @ 40F)</v>
       </c>
     </row>
     <row r="66" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C66" s="1">
-        <v>367</v>
+        <v>271</v>
       </c>
       <c r="D66" s="9">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E66" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E66" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-60-*-***C****  (11kW cap @ 40F)</v>
+        <v>A. O. Smith AHPA-250-*-***C****  (45kW cap @ 40F)</v>
       </c>
     </row>
     <row r="67" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C67" s="1">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D67" s="9">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="E67" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G67" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-90-*-***C****  (20kW cap @ 40F)</v>
+        <v>State SHPA-60-*-***C****  (11kW cap @ 40F)</v>
       </c>
     </row>
     <row r="68" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C68" s="1">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D68" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="E68" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E68" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F68" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-125-*-***C****  (26kW cap @ 40F)</v>
+        <v>State SHPA-90-*-***C****  (20kW cap @ 40F)</v>
       </c>
     </row>
     <row r="69" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C69" s="1">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D69" s="9">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="E69" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E69" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F69" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-185-*-***C****  (40kW cap @ 40F)</v>
+        <v>State SHPA-125-*-***C****  (26kW cap @ 40F)</v>
       </c>
     </row>
     <row r="70" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C70" s="1">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D70" s="9">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="E70" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E70" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F70" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="1"/>
-        <v>State SHPA-250-*-***C****  (45kW cap @ 40F)</v>
+        <v>State SHPA-185-*-***C****  (40kW cap @ 40F)</v>
       </c>
     </row>
     <row r="71" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C71" s="1">
-        <v>77</v>
+        <v>371</v>
       </c>
       <c r="D71" s="9">
-        <v>14</v>
-      </c>
-      <c r="E71" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F71" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="G71" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="H71" s="21" t="s">
-        <v>91</v>
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="E71" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F71" t="s">
+        <v>53</v>
+      </c>
+      <c r="G71" t="str">
+        <f t="shared" si="1"/>
+        <v>State SHPA-250-*-***C****  (45kW cap @ 40F)</v>
       </c>
     </row>
     <row r="72" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C72" s="1">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D72" s="9">
-        <v>21</v>
-      </c>
-      <c r="E72" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F72" t="s">
-        <v>81</v>
-      </c>
-      <c r="G72" t="s">
-        <v>92</v>
+        <v>14</v>
+      </c>
+      <c r="E72" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F72" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G72" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="H72" s="20" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="73" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C73" s="1">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D73" s="9">
-        <v>29</v>
-      </c>
-      <c r="E73" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G73" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="74" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C74" s="1">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D74" s="9">
-        <v>41</v>
-      </c>
-      <c r="E74" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E74" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F74" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G74" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="75" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C75" s="1">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D75" s="9">
-        <v>50</v>
-      </c>
-      <c r="E75" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E75" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F75" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G75" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C76" s="1">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D76" s="9">
-        <v>58</v>
-      </c>
-      <c r="E76" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E76" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F76" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G76" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="77" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C77" s="1">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D77" s="9">
-        <v>12</v>
-      </c>
-      <c r="E77" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E77" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F77" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G77" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="78" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C78" s="1">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D78" s="9">
         <v>12</v>
       </c>
-      <c r="E78" s="17" t="s">
+      <c r="E78" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F78" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G78" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C79" s="1">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D79" s="9">
-        <v>30</v>
-      </c>
-      <c r="E79" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F79" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G79" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="80" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C80" s="1">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D80" s="9">
         <v>30</v>
       </c>
-      <c r="E80" s="17" t="s">
+      <c r="E80" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F80" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G80" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C81" s="1">
-        <v>991</v>
+        <v>86</v>
       </c>
       <c r="D81" s="9">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E81" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F81" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="G81" s="21" t="str">
-        <f t="shared" si="1"/>
-        <v>generic  (5kW cap @ 40F)</v>
-      </c>
-      <c r="H81" s="21"/>
+        <v>30</v>
+      </c>
+      <c r="E81" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F81" t="s">
+        <v>87</v>
+      </c>
+      <c r="G81" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C82" s="1">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="D82" s="9">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E82" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F82" t="s">
+        <v>5</v>
+      </c>
+      <c r="E82" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F82" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="G82" t="str">
-        <f t="shared" si="1"/>
-        <v>generic  (11kW cap @ 40F)</v>
-      </c>
+      <c r="G82" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>generic  (5kW cap @ 40F)</v>
+      </c>
+      <c r="H82" s="20"/>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C83" s="1">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="D83" s="9">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="E83" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F83" t="s">
@@ -2508,18 +2556,18 @@
       </c>
       <c r="G83" t="str">
         <f t="shared" si="1"/>
-        <v>generic  (20kW cap @ 40F)</v>
+        <v>generic  (11kW cap @ 40F)</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C84" s="1">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="D84" s="9">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="E84" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E84" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F84" t="s">
@@ -2527,18 +2575,18 @@
       </c>
       <c r="G84" t="str">
         <f t="shared" si="1"/>
-        <v>generic  (26kW cap @ 40F)</v>
+        <v>generic  (20kW cap @ 40F)</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C85" s="1">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D85" s="9">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="E85" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E85" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F85" t="s">
@@ -2546,18 +2594,18 @@
       </c>
       <c r="G85" t="str">
         <f t="shared" si="1"/>
-        <v>generic  (40kW cap @ 40F)</v>
+        <v>generic  (26kW cap @ 40F)</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C86" s="1">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="D86" s="9">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="E86" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E86" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F86" t="s">
@@ -2565,30 +2613,50 @@
       </c>
       <c r="G86" t="str">
         <f t="shared" si="1"/>
+        <v>generic  (40kW cap @ 40F)</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C87" s="1">
+        <v>996</v>
+      </c>
+      <c r="D87" s="9">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="E87" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F87" t="s">
+        <v>79</v>
+      </c>
+      <c r="G87" t="str">
+        <f t="shared" si="1"/>
         <v>generic  (45kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C87" s="18" t="s">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C88" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D87" s="19">
-        <v>0</v>
-      </c>
-      <c r="E87" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="D88" s="18">
+        <v>0</v>
+      </c>
+      <c r="E88" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F88" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SVN Revision #7034 by scriswellwsf       ruleset &amp; CSE mods enabling multi pass compressors for primary and secondary central HPWH systems and restructuring inputs a bit for clarity
</commit_message>
<xml_diff>
--- a/Documentation/T24N/T24R_CentralHPWHCompressors.xlsx
+++ b/Documentation/T24N/T24R_CentralHPWHCompressors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Com\branches\CBECC-Com_MFamRestructure\Documentation\T24N\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19B5DED-5603-40B8-8218-A38C307FE38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6EB2F5-6517-4155-96F6-23BD60DE0313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="390" windowWidth="28155" windowHeight="12885" xr2:uid="{06DD2E85-E74E-41DF-AAE4-37E8BABFD5C8}"/>
+    <workbookView xWindow="4665" yWindow="870" windowWidth="23205" windowHeight="12180" xr2:uid="{06DD2E85-E74E-41DF-AAE4-37E8BABFD5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <author>Scott Criswell</author>
   </authors>
   <commentList>
-    <comment ref="K14" authorId="0" shapeId="0" xr:uid="{6303DEEF-C866-46FF-8A24-CA09C6A7EC95}">
+    <comment ref="K15" authorId="0" shapeId="0" xr:uid="{6303DEEF-C866-46FF-8A24-CA09C6A7EC95}">
       <text>
         <r>
           <rPr>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="157">
   <si>
     <t>;</t>
   </si>
@@ -378,10 +378,166 @@
     <t>01/18/22 - SAC - added multi pass compressor types</t>
   </si>
   <si>
-    <t>02/03/22 - SAC</t>
-  </si>
-  <si>
     <t>02/03/22 - SAC - updated Colmac CxV-5 compressor OutputCap from 10 to 14 kW</t>
+  </si>
+  <si>
+    <t>more multi pass options - SAC 02/23/22</t>
+  </si>
+  <si>
+    <t>Nyle C60A  (MP)</t>
+  </si>
+  <si>
+    <t>Nyle C90A  (MP)</t>
+  </si>
+  <si>
+    <t>Nyle C125A  (MP)</t>
+  </si>
+  <si>
+    <t>Nyle C185A  (MP)</t>
+  </si>
+  <si>
+    <t>Nyle C250A  (MP)</t>
+  </si>
+  <si>
+    <t>Nyle C60A-CWP  (MP)</t>
+  </si>
+  <si>
+    <t>Nyle C90A-CWP  (MP)</t>
+  </si>
+  <si>
+    <t>Nyle C125A-CWP  (MP)</t>
+  </si>
+  <si>
+    <t>Nyle C185A-CWP  (MP)</t>
+  </si>
+  <si>
+    <t>Nyle C250A-CWP  (MP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nyle C60A  (MP, 11kw cap @ 40F)   </t>
+  </si>
+  <si>
+    <t>Nyle C90A  (MP, 20kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Nyle C125A  (MP, 26kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Nyle C185A  (MP, 41kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Nyle C250A  (MP, 46kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Nyle C60A-C  (MP, 11kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Nyle C90A-C  (MP, 20kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Nyle C125A-C  (MP, 26kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Nyle C185A-C  (MP, 41kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Nyle C250A-C  (MP, 46kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Lochinvar AHP060-*-***N****  (MP, 11kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Lochinvar AHP090-*-***N****  (MP, 20kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Lochinvar AHP125-*-***N****  (MP, 26kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Lochinvar AHP185-*-***N****  (MP, 41kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Lochinvar AHP250-*-***N****  (MP, 46kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>A. O. Smith AHPA-60-*-***N****  (MP, 11kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>A. O. Smith AHPA-90-*-***N****  (MP, 20kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>A. O. Smith AHPA-125-*-***N****  (MP, 26kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>A. O. Smith AHPA-185-*-***N****  (MP, 41kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>A. O. Smith AHPA-250-*-***N****  (MP, 46kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>State SHPA-60-*-***N****  (MP, 11kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>State SHPA-90-*-***N****  (MP, 20kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>State SHPA-125-*-***N****  (MP, 26kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>State SHPA-185-*-***N****  (MP, 41kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>State SHPA-250-*-***N****  (MP, 46kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Lochinvar AHP060-*-***C****  (MP, 11kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Lochinvar AHP090-*-***C****  (MP, 20kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Lochinvar AHP125-*-***C****  (MP, 26kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Lochinvar AHP185-*-***C****  (MP, 41kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>Lochinvar AHP250-*-***C****  (MP, 46kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>A. O. Smith AHPA-60-*-***C****  (MP, 11kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>A. O. Smith AHPA-90-*-***C****  (MP, 20kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>A. O. Smith AHPA-125-*-***C****  (MP, 26kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>A. O. Smith AHPA-185-*-***C****  (MP, 41kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>A. O. Smith AHPA-250-*-***C****  (MP, 46kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>State SHPA-60-*-***C****  (MP, 11kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>State SHPA-90-*-***C****  (MP, 20kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>State SHPA-125-*-***C****  (MP, 26kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>State SHPA-185-*-***C****  (MP, 41kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>State SHPA-250-*-***C****  (MP, 46kw cap @ 40F)</t>
+  </si>
+  <si>
+    <t>02/23/22 - SAC - added Nyle multi pass compressor types</t>
+  </si>
+  <si>
+    <t>02/23/22 - SAC</t>
   </si>
 </sst>
 </file>
@@ -946,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD161AC-8F54-43FE-9249-2CA51C7B791C}">
-  <dimension ref="A1:K89"/>
+  <dimension ref="A1:K130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,7 +1116,7 @@
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="2.85546875" customWidth="1"/>
     <col min="6" max="6" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.5703125" customWidth="1"/>
+    <col min="7" max="7" width="49.7109375" customWidth="1"/>
     <col min="8" max="8" width="4.28515625" customWidth="1"/>
     <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -990,7 +1146,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1022,7 +1178,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>104</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1030,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1038,7 +1194,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1046,113 +1202,106 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>77</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>12</v>
-      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="I14" s="9">
-        <v>48</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K14" s="21">
-        <v>14</v>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
       <c r="C15" s="1"/>
       <c r="I15" s="9">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" s="21">
         <v>14</v>
-      </c>
-      <c r="K15" s="10">
-        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>78</v>
-      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="I16" s="9">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K16" s="10">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>78</v>
+      </c>
       <c r="I17" s="9">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K17" s="10">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1160,417 +1309,402 @@
         <v>0</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
       <c r="I18" s="9">
+        <v>45</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" s="10">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="I19" s="9">
         <v>51</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K19" s="10">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="I19" s="9">
+      <c r="D20" s="2"/>
+      <c r="I20" s="9">
         <v>52</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K20" s="10">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="3" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="3" t="s">
+      <c r="E21" s="5"/>
+      <c r="F21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I21" s="9">
         <v>53</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K21" s="10">
         <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C21" s="1">
-        <v>48</v>
-      </c>
-      <c r="D21" s="22">
-        <f t="shared" ref="D21:D87" si="0">VLOOKUP( MOD(C21,100), $I$14:$K$40, 3, FALSE )</f>
-        <v>14</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" t="str">
-        <f xml:space="preserve"> F21 &amp; "  (" &amp; D21 &amp; "kW cap @ 40F)"</f>
-        <v>Colmac CxV-5  (14kW cap @ 40F)</v>
-      </c>
-      <c r="I21" s="9">
-        <v>54</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K21" s="10">
-        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
-        <v>49</v>
-      </c>
-      <c r="D22" s="9">
-        <f t="shared" si="0"/>
-        <v>21</v>
+        <v>48</v>
+      </c>
+      <c r="D22" s="22">
+        <f>VLOOKUP( MOD(C22,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>14</v>
       </c>
       <c r="E22" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" ref="G22:G87" si="1" xml:space="preserve"> F22 &amp; "  (" &amp; D22 &amp; "kW cap @ 40F)"</f>
-        <v>Colmac CxA-10  (21kW cap @ 40F)</v>
+        <f xml:space="preserve"> F22 &amp; "  (" &amp; D22 &amp; "kW cap @ 40F)"</f>
+        <v>Colmac CxV-5  (14kW cap @ 40F)</v>
       </c>
       <c r="I22" s="9">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K22" s="10">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="9">
-        <f t="shared" si="0"/>
-        <v>29</v>
+        <f>VLOOKUP( MOD(C23,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>21</v>
       </c>
       <c r="E23" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="1"/>
-        <v>Colmac CxA-15  (29kW cap @ 40F)</v>
+        <f t="shared" ref="G23:G128" si="0" xml:space="preserve"> F23 &amp; "  (" &amp; D23 &amp; "kW cap @ 40F)"</f>
+        <v>Colmac CxA-10  (21kW cap @ 40F)</v>
       </c>
       <c r="I23" s="9">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K23" s="10">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D24" s="9">
-        <f t="shared" si="0"/>
-        <v>41</v>
+        <f>VLOOKUP( MOD(C24,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>29</v>
       </c>
       <c r="E24" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="1"/>
-        <v>Colmac CxA-20  (41kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>Colmac CxA-15  (29kW cap @ 40F)</v>
       </c>
       <c r="I24" s="9">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K24" s="10">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D25" s="9">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <f>VLOOKUP( MOD(C25,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>41</v>
       </c>
       <c r="E25" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="1"/>
-        <v>Colmac CxA-25  (49kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>Colmac CxA-20  (41kW cap @ 40F)</v>
       </c>
       <c r="I25" s="9">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K25" s="10">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D26" s="9">
-        <f t="shared" si="0"/>
-        <v>57</v>
+        <f>VLOOKUP( MOD(C26,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>49</v>
       </c>
       <c r="E26" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="1"/>
-        <v>Colmac CxA-30  (57kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>Colmac CxA-25  (49kW cap @ 40F)</v>
       </c>
       <c r="I26" s="9">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K26" s="10">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D27" s="9">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>VLOOKUP( MOD(C27,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>57</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="1"/>
-        <v>Nyle C25A  (5kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>Colmac CxA-30  (57kW cap @ 40F)</v>
       </c>
       <c r="I27" s="9">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K27" s="10">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D28" s="9">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f>VLOOKUP( MOD(C28,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>5</v>
       </c>
       <c r="E28" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>Nyle C25A  (5kW cap @ 40F)</v>
+      </c>
+      <c r="I28" s="9">
+        <v>68</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K28" s="10">
         <v>20</v>
-      </c>
-      <c r="G28" t="str">
-        <f t="shared" si="1"/>
-        <v>Nyle C60A  (11kW cap @ 40F)</v>
-      </c>
-      <c r="I28" s="9">
-        <v>69</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K28" s="10">
-        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" s="9">
-        <f t="shared" si="0"/>
+        <f>VLOOKUP( MOD(C29,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>11</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F29" t="s">
-        <v>21</v>
-      </c>
       <c r="G29" t="str">
-        <f t="shared" si="1"/>
-        <v>Nyle C90A  (20kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>Nyle C60A  (11kW cap @ 40F)</v>
       </c>
       <c r="I29" s="9">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K29" s="10">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D30" s="9">
-        <f t="shared" si="0"/>
-        <v>26</v>
+        <f>VLOOKUP( MOD(C30,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>20</v>
       </c>
       <c r="E30" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="1"/>
-        <v>Nyle C125A  (26kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>Nyle C90A  (20kW cap @ 40F)</v>
       </c>
       <c r="I30" s="9">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K30" s="10">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D31" s="9">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f>VLOOKUP( MOD(C31,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>26</v>
       </c>
       <c r="E31" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="1"/>
-        <v>Nyle C185A  (40kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>Nyle C125A  (26kW cap @ 40F)</v>
       </c>
       <c r="I31" s="9">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K31" s="10">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D32" s="9">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <f>VLOOKUP( MOD(C32,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>40</v>
       </c>
       <c r="E32" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="1"/>
-        <v>Nyle C250A  (45kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>Nyle C185A  (40kW cap @ 40F)</v>
       </c>
       <c r="I32" s="9">
-        <v>91</v>
-      </c>
-      <c r="J32" s="19" t="str">
-        <f>"Generic-" &amp; K32</f>
-        <v>Generic-5</v>
+        <v>57</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="K32" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="D33" s="9">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f>VLOOKUP( MOD(C33,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>45</v>
       </c>
       <c r="E33" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="1"/>
-        <v>Nyle C60A-C  (11kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>Nyle C250A  (45kW cap @ 40F)</v>
       </c>
       <c r="I33" s="9">
-        <v>92</v>
-      </c>
-      <c r="J33" s="19" t="str">
-        <f t="shared" ref="J33:J37" si="2">"Generic-" &amp; K33</f>
-        <v>Generic-11</v>
+        <v>5</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="K33" s="10">
         <v>11</v>
@@ -1578,28 +1712,27 @@
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D34" s="9">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>VLOOKUP( MOD(C34,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>11</v>
       </c>
       <c r="E34" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="1"/>
-        <v>Nyle C90A-C  (20kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>Nyle C60A-C  (11kW cap @ 40F)</v>
       </c>
       <c r="I34" s="9">
-        <v>93</v>
-      </c>
-      <c r="J34" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>Generic-20</v>
+        <v>6</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>106</v>
       </c>
       <c r="K34" s="10">
         <v>20</v>
@@ -1607,28 +1740,27 @@
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D35" s="9">
-        <f t="shared" si="0"/>
-        <v>26</v>
+        <f>VLOOKUP( MOD(C35,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>20</v>
       </c>
       <c r="E35" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="1"/>
-        <v>Nyle C125A-C  (26kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>Nyle C90A-C  (20kW cap @ 40F)</v>
       </c>
       <c r="I35" s="9">
-        <v>94</v>
-      </c>
-      <c r="J35" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>Generic-26</v>
+        <v>7</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>107</v>
       </c>
       <c r="K35" s="10">
         <v>26</v>
@@ -1636,842 +1768,947 @@
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D36" s="9">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f>VLOOKUP( MOD(C36,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>26</v>
       </c>
       <c r="E36" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="1"/>
-        <v>Nyle C185A-C  (40kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>Nyle C125A-C  (26kW cap @ 40F)</v>
       </c>
       <c r="I36" s="9">
-        <v>95</v>
-      </c>
-      <c r="J36" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>Generic-40</v>
+        <v>8</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="K36" s="10">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D37" s="9">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <f>VLOOKUP( MOD(C37,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>40</v>
       </c>
       <c r="E37" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="1"/>
-        <v>Nyle C250A-C  (45kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>Nyle C185A-C  (40kW cap @ 40F)</v>
       </c>
       <c r="I37" s="9">
-        <v>96</v>
-      </c>
-      <c r="J37" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v>Generic-45</v>
+        <v>9</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="K37" s="10">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="D38" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>VLOOKUP( MOD(C38,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>45</v>
       </c>
       <c r="E38" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="1"/>
-        <v>Sanden GS3-45HPA-US  (4kW cap @ 40F)</v>
-      </c>
-      <c r="I38" s="9"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="10"/>
+        <f t="shared" si="0"/>
+        <v>Nyle C250A-C  (45kW cap @ 40F)</v>
+      </c>
+      <c r="I38" s="9">
+        <v>25</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="K38" s="10">
+        <v>11</v>
+      </c>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
-        <v>153</v>
+        <v>57</v>
       </c>
       <c r="D39" s="9">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>VLOOKUP( MOD(C39,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>4</v>
       </c>
       <c r="E39" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="1"/>
-        <v>Lochinvar AHP025-*-***N****  (5kW cap @ 40F)</v>
-      </c>
-      <c r="I39" s="9"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="10"/>
+        <f t="shared" si="0"/>
+        <v>Sanden GS3-45HPA-US  (4kW cap @ 40F)</v>
+      </c>
+      <c r="I39" s="9">
+        <v>26</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="K39" s="10">
+        <v>20</v>
+      </c>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D40" s="9">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f>VLOOKUP( MOD(C40,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>5</v>
       </c>
       <c r="E40" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="1"/>
-        <v>Lochinvar AHP060-*-***N****  (11kW cap @ 40F)</v>
-      </c>
-      <c r="I40" s="11"/>
-      <c r="J40" s="12"/>
-      <c r="K40" s="13"/>
+        <f t="shared" si="0"/>
+        <v>Lochinvar AHP025-*-***N****  (5kW cap @ 40F)</v>
+      </c>
+      <c r="I40" s="9">
+        <v>27</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="K40" s="10">
+        <v>26</v>
+      </c>
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D41" s="9">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>VLOOKUP( MOD(C41,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>11</v>
       </c>
       <c r="E41" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F41" t="s">
+        <v>40</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v>Lochinvar AHP060-*-***N****  (11kW cap @ 40F)</v>
+      </c>
+      <c r="I41" s="9">
+        <v>28</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K41" s="10">
         <v>41</v>
-      </c>
-      <c r="G41" t="str">
-        <f t="shared" si="1"/>
-        <v>Lochinvar AHP090-*-***N****  (20kW cap @ 40F)</v>
       </c>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D42" s="9">
-        <f t="shared" si="0"/>
-        <v>26</v>
+        <f>VLOOKUP( MOD(C42,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>20</v>
       </c>
       <c r="E42" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="1"/>
-        <v>Lochinvar AHP125-*-***N****  (26kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>Lochinvar AHP090-*-***N****  (20kW cap @ 40F)</v>
+      </c>
+      <c r="I42" s="9">
+        <v>29</v>
+      </c>
+      <c r="J42" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K42" s="10">
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="D43" s="9">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f>VLOOKUP( MOD(C43,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>26</v>
       </c>
       <c r="E43" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="1"/>
-        <v>Lochinvar AHP185-*-***N****  (40kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>Lochinvar AHP125-*-***N****  (26kW cap @ 40F)</v>
+      </c>
+      <c r="I43" s="9">
+        <v>91</v>
+      </c>
+      <c r="J43" s="19" t="str">
+        <f>"Generic-" &amp; K43</f>
+        <v>Generic-5</v>
+      </c>
+      <c r="K43" s="10">
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D44" s="9">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <f>VLOOKUP( MOD(C44,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>40</v>
       </c>
       <c r="E44" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="1"/>
-        <v>Lochinvar AHP250-*-***N****  (45kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>Lochinvar AHP185-*-***N****  (40kW cap @ 40F)</v>
+      </c>
+      <c r="I44" s="9">
+        <v>92</v>
+      </c>
+      <c r="J44" s="19" t="str">
+        <f t="shared" ref="J44:J48" si="1">"Generic-" &amp; K44</f>
+        <v>Generic-11</v>
+      </c>
+      <c r="K44" s="10">
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
-        <v>253</v>
+        <v>147</v>
       </c>
       <c r="D45" s="9">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>VLOOKUP( MOD(C45,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>45</v>
       </c>
       <c r="E45" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G45" t="str">
+        <f t="shared" si="0"/>
+        <v>Lochinvar AHP250-*-***N****  (45kW cap @ 40F)</v>
+      </c>
+      <c r="I45" s="9">
+        <v>93</v>
+      </c>
+      <c r="J45" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-25-*-***N****  (5kW cap @ 40F)</v>
+        <v>Generic-20</v>
+      </c>
+      <c r="K45" s="10">
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D46" s="9">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f>VLOOKUP( MOD(C46,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>5</v>
       </c>
       <c r="E46" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G46" t="str">
+        <f t="shared" si="0"/>
+        <v>A. O. Smith AHPA-25-*-***N****  (5kW cap @ 40F)</v>
+      </c>
+      <c r="I46" s="9">
+        <v>94</v>
+      </c>
+      <c r="J46" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-60-*-***N****  (11kW cap @ 40F)</v>
+        <v>Generic-26</v>
+      </c>
+      <c r="K46" s="10">
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D47" s="9">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>VLOOKUP( MOD(C47,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>11</v>
       </c>
       <c r="E47" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G47" t="str">
+        <f t="shared" si="0"/>
+        <v>A. O. Smith AHPA-60-*-***N****  (11kW cap @ 40F)</v>
+      </c>
+      <c r="I47" s="9">
+        <v>95</v>
+      </c>
+      <c r="J47" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-90-*-***N****  (20kW cap @ 40F)</v>
+        <v>Generic-40</v>
+      </c>
+      <c r="K47" s="10">
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
+        <v>255</v>
+      </c>
+      <c r="D48" s="9">
+        <f>VLOOKUP( MOD(C48,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>20</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>56</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="0"/>
+        <v>A. O. Smith AHPA-90-*-***N****  (20kW cap @ 40F)</v>
+      </c>
+      <c r="I48" s="9">
+        <v>96</v>
+      </c>
+      <c r="J48" s="19" t="str">
+        <f t="shared" si="1"/>
+        <v>Generic-45</v>
+      </c>
+      <c r="K48" s="10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C49" s="1">
         <v>256</v>
       </c>
-      <c r="D48" s="9">
-        <f t="shared" si="0"/>
+      <c r="D49" s="9">
+        <f>VLOOKUP( MOD(C49,100), $I$15:$K$51, 3, FALSE )</f>
         <v>26</v>
       </c>
-      <c r="E48" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="E49" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F49" t="s">
         <v>45</v>
       </c>
-      <c r="G48" t="str">
-        <f t="shared" si="1"/>
+      <c r="G49" t="str">
+        <f t="shared" si="0"/>
         <v>A. O. Smith AHPA-125-*-***N****  (26kW cap @ 40F)</v>
       </c>
-    </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C49" s="1">
+      <c r="I49" s="9"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="10"/>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C50" s="1">
         <v>246</v>
       </c>
-      <c r="D49" s="9">
-        <f t="shared" si="0"/>
+      <c r="D50" s="9">
+        <f>VLOOKUP( MOD(C50,100), $I$15:$K$51, 3, FALSE )</f>
         <v>40</v>
       </c>
-      <c r="E49" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F49" t="s">
+      <c r="E50" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F50" t="s">
         <v>46</v>
       </c>
-      <c r="G49" t="str">
-        <f t="shared" si="1"/>
+      <c r="G50" t="str">
+        <f t="shared" si="0"/>
         <v>A. O. Smith AHPA-185-*-***N****  (40kW cap @ 40F)</v>
       </c>
-    </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C50" s="1">
+      <c r="I50" s="9"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="10"/>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C51" s="1">
         <v>247</v>
       </c>
-      <c r="D50" s="9">
-        <f t="shared" si="0"/>
+      <c r="D51" s="9">
+        <f>VLOOKUP( MOD(C51,100), $I$15:$K$51, 3, FALSE )</f>
         <v>45</v>
       </c>
-      <c r="E50" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="E51" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
         <v>47</v>
       </c>
-      <c r="G50" t="str">
-        <f t="shared" si="1"/>
+      <c r="G51" t="str">
+        <f t="shared" si="0"/>
         <v>A. O. Smith AHPA-250-*-***N****  (45kW cap @ 40F)</v>
       </c>
-    </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C51" s="1">
+      <c r="I51" s="11"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="13"/>
+    </row>
+    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C52" s="1">
         <v>353</v>
       </c>
-      <c r="D51" s="9">
-        <f t="shared" si="0"/>
+      <c r="D52" s="9">
+        <f>VLOOKUP( MOD(C52,100), $I$15:$K$51, 3, FALSE )</f>
         <v>5</v>
       </c>
-      <c r="E51" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F51" t="s">
+      <c r="E52" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F52" t="s">
         <v>57</v>
       </c>
-      <c r="G51" t="str">
-        <f t="shared" si="1"/>
+      <c r="G52" t="str">
+        <f t="shared" si="0"/>
         <v>State SHPA-25-*-***N****  (5kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="1">
+    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C53" s="1">
         <v>354</v>
       </c>
-      <c r="D52" s="9">
-        <f t="shared" si="0"/>
+      <c r="D53" s="9">
+        <f>VLOOKUP( MOD(C53,100), $I$15:$K$51, 3, FALSE )</f>
         <v>11</v>
       </c>
-      <c r="E52" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F52" t="s">
+      <c r="E53" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F53" t="s">
         <v>58</v>
       </c>
-      <c r="G52" t="str">
-        <f t="shared" si="1"/>
+      <c r="G53" t="str">
+        <f t="shared" si="0"/>
         <v>State SHPA-60-*-***N****  (11kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C53" s="1">
+    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C54" s="1">
         <v>355</v>
       </c>
-      <c r="D53" s="9">
-        <f t="shared" si="0"/>
+      <c r="D54" s="9">
+        <f>VLOOKUP( MOD(C54,100), $I$15:$K$51, 3, FALSE )</f>
         <v>20</v>
       </c>
-      <c r="E53" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="E54" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F54" t="s">
         <v>59</v>
       </c>
-      <c r="G53" t="str">
-        <f t="shared" si="1"/>
+      <c r="G54" t="str">
+        <f t="shared" si="0"/>
         <v>State SHPA-90-*-***N****  (20kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C54" s="1">
+    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C55" s="1">
         <v>356</v>
       </c>
-      <c r="D54" s="9">
-        <f t="shared" si="0"/>
+      <c r="D55" s="9">
+        <f>VLOOKUP( MOD(C55,100), $I$15:$K$51, 3, FALSE )</f>
         <v>26</v>
       </c>
-      <c r="E54" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F54" t="s">
+      <c r="E55" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F55" t="s">
         <v>60</v>
       </c>
-      <c r="G54" t="str">
-        <f t="shared" si="1"/>
+      <c r="G55" t="str">
+        <f t="shared" si="0"/>
         <v>State SHPA-125-*-***N****  (26kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C55" s="1">
+    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C56" s="1">
         <v>346</v>
       </c>
-      <c r="D55" s="9">
-        <f t="shared" si="0"/>
+      <c r="D56" s="9">
+        <f>VLOOKUP( MOD(C56,100), $I$15:$K$51, 3, FALSE )</f>
         <v>40</v>
       </c>
-      <c r="E55" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="E56" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F56" t="s">
         <v>61</v>
       </c>
-      <c r="G55" t="str">
-        <f t="shared" si="1"/>
+      <c r="G56" t="str">
+        <f t="shared" si="0"/>
         <v>State SHPA-185-*-***N****  (40kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C56" s="1">
+    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C57" s="1">
         <v>347</v>
       </c>
-      <c r="D56" s="9">
-        <f t="shared" si="0"/>
+      <c r="D57" s="9">
+        <f>VLOOKUP( MOD(C57,100), $I$15:$K$51, 3, FALSE )</f>
         <v>45</v>
       </c>
-      <c r="E56" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="E57" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F57" t="s">
         <v>62</v>
       </c>
-      <c r="G56" t="str">
-        <f t="shared" si="1"/>
+      <c r="G57" t="str">
+        <f t="shared" si="0"/>
         <v>State SHPA-250-*-***N****  (45kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C57" s="1">
+    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C58" s="1">
         <v>167</v>
       </c>
-      <c r="D57" s="9">
-        <f t="shared" si="0"/>
+      <c r="D58" s="9">
+        <f>VLOOKUP( MOD(C58,100), $I$15:$K$51, 3, FALSE )</f>
         <v>11</v>
       </c>
-      <c r="E57" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F57" t="s">
+      <c r="E58" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F58" t="s">
         <v>63</v>
       </c>
-      <c r="G57" t="str">
-        <f t="shared" si="1"/>
+      <c r="G58" t="str">
+        <f t="shared" si="0"/>
         <v>Lochinvar AHP060-*-***C****  (11kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C58" s="1">
+    <row r="59" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C59" s="1">
         <v>168</v>
       </c>
-      <c r="D58" s="9">
-        <f t="shared" si="0"/>
+      <c r="D59" s="9">
+        <f>VLOOKUP( MOD(C59,100), $I$15:$K$51, 3, FALSE )</f>
         <v>20</v>
       </c>
-      <c r="E58" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="E59" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F59" t="s">
         <v>64</v>
       </c>
-      <c r="G58" t="str">
-        <f t="shared" si="1"/>
+      <c r="G59" t="str">
+        <f t="shared" si="0"/>
         <v>Lochinvar AHP090-*-***C****  (20kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="1">
+    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C60" s="1">
         <v>169</v>
       </c>
-      <c r="D59" s="9">
-        <f t="shared" si="0"/>
+      <c r="D60" s="9">
+        <f>VLOOKUP( MOD(C60,100), $I$15:$K$51, 3, FALSE )</f>
         <v>26</v>
       </c>
-      <c r="E59" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="E60" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F60" t="s">
         <v>65</v>
       </c>
-      <c r="G59" t="str">
-        <f t="shared" si="1"/>
+      <c r="G60" t="str">
+        <f t="shared" si="0"/>
         <v>Lochinvar AHP125-*-***C****  (26kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C60" s="1">
+    <row r="61" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C61" s="1">
         <v>170</v>
       </c>
-      <c r="D60" s="9">
-        <f t="shared" si="0"/>
+      <c r="D61" s="9">
+        <f>VLOOKUP( MOD(C61,100), $I$15:$K$51, 3, FALSE )</f>
         <v>40</v>
       </c>
-      <c r="E60" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F60" t="s">
+      <c r="E61" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F61" t="s">
         <v>66</v>
       </c>
-      <c r="G60" t="str">
-        <f t="shared" si="1"/>
+      <c r="G61" t="str">
+        <f t="shared" si="0"/>
         <v>Lochinvar AHP185-*-***C****  (40kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C61" s="1">
+    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C62" s="1">
         <v>171</v>
       </c>
-      <c r="D61" s="9">
-        <f t="shared" si="0"/>
+      <c r="D62" s="9">
+        <f>VLOOKUP( MOD(C62,100), $I$15:$K$51, 3, FALSE )</f>
         <v>45</v>
       </c>
-      <c r="E61" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F61" t="s">
+      <c r="E62" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F62" t="s">
         <v>67</v>
       </c>
-      <c r="G61" t="str">
-        <f t="shared" si="1"/>
+      <c r="G62" t="str">
+        <f t="shared" si="0"/>
         <v>Lochinvar AHP250-*-***C****  (45kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="1">
+    <row r="63" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C63" s="1">
         <v>267</v>
       </c>
-      <c r="D62" s="9">
-        <f t="shared" si="0"/>
+      <c r="D63" s="9">
+        <f>VLOOKUP( MOD(C63,100), $I$15:$K$51, 3, FALSE )</f>
         <v>11</v>
       </c>
-      <c r="E62" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="E63" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F63" t="s">
         <v>68</v>
       </c>
-      <c r="G62" t="str">
-        <f t="shared" si="1"/>
+      <c r="G63" t="str">
+        <f t="shared" si="0"/>
         <v>A. O. Smith AHPA-60-*-***C****  (11kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C63" s="1">
+    <row r="64" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C64" s="1">
         <v>268</v>
       </c>
-      <c r="D63" s="9">
-        <f t="shared" si="0"/>
+      <c r="D64" s="9">
+        <f>VLOOKUP( MOD(C64,100), $I$15:$K$51, 3, FALSE )</f>
         <v>20</v>
       </c>
-      <c r="E63" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="E64" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F64" t="s">
         <v>69</v>
       </c>
-      <c r="G63" t="str">
-        <f t="shared" si="1"/>
+      <c r="G64" t="str">
+        <f t="shared" si="0"/>
         <v>A. O. Smith AHPA-90-*-***C****  (20kW cap @ 40F)</v>
-      </c>
-    </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C64" s="1">
-        <v>269</v>
-      </c>
-      <c r="D64" s="9">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="E64" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F64" t="s">
-        <v>48</v>
-      </c>
-      <c r="G64" t="str">
-        <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-125-*-***C****  (26kW cap @ 40F)</v>
       </c>
     </row>
     <row r="65" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C65" s="1">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D65" s="9">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f>VLOOKUP( MOD(C65,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>26</v>
       </c>
       <c r="E65" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G65" t="str">
-        <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-185-*-***C****  (40kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>A. O. Smith AHPA-125-*-***C****  (26kW cap @ 40F)</v>
       </c>
     </row>
     <row r="66" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C66" s="1">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D66" s="9">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <f>VLOOKUP( MOD(C66,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>40</v>
       </c>
       <c r="E66" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" si="1"/>
-        <v>A. O. Smith AHPA-250-*-***C****  (45kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>A. O. Smith AHPA-185-*-***C****  (40kW cap @ 40F)</v>
       </c>
     </row>
     <row r="67" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C67" s="1">
-        <v>367</v>
+        <v>271</v>
       </c>
       <c r="D67" s="9">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f>VLOOKUP( MOD(C67,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>45</v>
       </c>
       <c r="E67" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F67" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" si="1"/>
-        <v>State SHPA-60-*-***C****  (11kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>A. O. Smith AHPA-250-*-***C****  (45kW cap @ 40F)</v>
       </c>
     </row>
     <row r="68" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C68" s="1">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D68" s="9">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>VLOOKUP( MOD(C68,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>11</v>
       </c>
       <c r="E68" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G68" t="str">
-        <f t="shared" si="1"/>
-        <v>State SHPA-90-*-***C****  (20kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>State SHPA-60-*-***C****  (11kW cap @ 40F)</v>
       </c>
     </row>
     <row r="69" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C69" s="1">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D69" s="9">
-        <f t="shared" si="0"/>
-        <v>26</v>
+        <f>VLOOKUP( MOD(C69,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>20</v>
       </c>
       <c r="E69" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F69" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="G69" t="str">
-        <f t="shared" si="1"/>
-        <v>State SHPA-125-*-***C****  (26kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>State SHPA-90-*-***C****  (20kW cap @ 40F)</v>
       </c>
     </row>
     <row r="70" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C70" s="1">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D70" s="9">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f>VLOOKUP( MOD(C70,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>26</v>
       </c>
       <c r="E70" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F70" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G70" t="str">
-        <f t="shared" si="1"/>
-        <v>State SHPA-185-*-***C****  (40kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>State SHPA-125-*-***C****  (26kW cap @ 40F)</v>
       </c>
     </row>
     <row r="71" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C71" s="1">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D71" s="9">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <f>VLOOKUP( MOD(C71,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>40</v>
       </c>
       <c r="E71" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F71" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="1"/>
-        <v>State SHPA-250-*-***C****  (45kW cap @ 40F)</v>
+        <f t="shared" si="0"/>
+        <v>State SHPA-185-*-***C****  (40kW cap @ 40F)</v>
       </c>
     </row>
     <row r="72" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C72" s="1">
-        <v>77</v>
+        <v>371</v>
       </c>
       <c r="D72" s="9">
-        <v>14</v>
+        <f>VLOOKUP( MOD(C72,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>45</v>
       </c>
       <c r="E72" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="F72" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="G72" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="H72" s="20" t="s">
-        <v>91</v>
+      <c r="F72" t="s">
+        <v>53</v>
+      </c>
+      <c r="G72" t="str">
+        <f t="shared" si="0"/>
+        <v>State SHPA-250-*-***C****  (45kW cap @ 40F)</v>
       </c>
     </row>
     <row r="73" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C73" s="1">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D73" s="9">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E73" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="F73" t="s">
-        <v>81</v>
-      </c>
-      <c r="G73" t="s">
-        <v>92</v>
+      <c r="F73" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G73" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="H73" s="20" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="74" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C74" s="1">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D74" s="9">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E74" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F74" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G74" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="75" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C75" s="1">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D75" s="9">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E75" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F75" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G75" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="76" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C76" s="1">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D76" s="9">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E76" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F76" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G76" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="77" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C77" s="1">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D77" s="9">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E77" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F77" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G77" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C78" s="1">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D78" s="9">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="E78" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F78" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G78" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C79" s="1">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D79" s="9">
         <v>12</v>
@@ -2480,32 +2717,32 @@
         <v>0</v>
       </c>
       <c r="F79" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G79" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C80" s="1">
+        <v>84</v>
+      </c>
+      <c r="D80" s="9">
+        <v>12</v>
+      </c>
+      <c r="E80" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F80" t="s">
+        <v>89</v>
+      </c>
+      <c r="G80" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C81" s="1">
         <v>85</v>
-      </c>
-      <c r="D80" s="9">
-        <v>30</v>
-      </c>
-      <c r="E80" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F80" t="s">
-        <v>90</v>
-      </c>
-      <c r="G80" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C81" s="1">
-        <v>86</v>
       </c>
       <c r="D81" s="9">
         <v>30</v>
@@ -2514,143 +2751,763 @@
         <v>0</v>
       </c>
       <c r="F81" t="s">
+        <v>90</v>
+      </c>
+      <c r="G81" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C82" s="1">
+        <v>86</v>
+      </c>
+      <c r="D82" s="9">
+        <v>30</v>
+      </c>
+      <c r="E82" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F82" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G82" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C82" s="1">
+    <row r="83" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C83" s="1">
+        <v>5</v>
+      </c>
+      <c r="D83" s="9">
+        <f>VLOOKUP( MOD(C83,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>11</v>
+      </c>
+      <c r="E83" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G83" t="s">
+        <v>115</v>
+      </c>
+      <c r="H83" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C84" s="1">
+        <v>6</v>
+      </c>
+      <c r="D84" s="9">
+        <f t="shared" ref="D84:D122" si="2">VLOOKUP( MOD(C84,100), $I$15:$K$51, 3, FALSE )</f>
+        <v>20</v>
+      </c>
+      <c r="E84" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G84" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="85" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C85" s="1">
+        <v>7</v>
+      </c>
+      <c r="D85" s="9">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="E85" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G85" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="86" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C86" s="1">
+        <v>8</v>
+      </c>
+      <c r="D86" s="9">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="E86" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G86" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C87" s="1">
+        <v>9</v>
+      </c>
+      <c r="D87" s="9">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="E87" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G87" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="88" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C88" s="1">
+        <v>25</v>
+      </c>
+      <c r="D88" s="9">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E88" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G88" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="89" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C89" s="1">
+        <v>26</v>
+      </c>
+      <c r="D89" s="9">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E89" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G89" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C90" s="1">
+        <v>27</v>
+      </c>
+      <c r="D90" s="9">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="E90" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G90" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="91" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C91" s="1">
+        <v>28</v>
+      </c>
+      <c r="D91" s="9">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="E91" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G91" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C92" s="1">
+        <v>29</v>
+      </c>
+      <c r="D92" s="9">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="E92" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G92" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="93" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C93" s="1">
+        <v>105</v>
+      </c>
+      <c r="D93" s="9">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E93" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G93" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="94" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C94" s="1">
+        <v>106</v>
+      </c>
+      <c r="D94" s="9">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E94" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G94" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="95" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C95" s="1">
+        <v>107</v>
+      </c>
+      <c r="D95" s="9">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="E95" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G95" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="96" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C96" s="1">
+        <v>108</v>
+      </c>
+      <c r="D96" s="9">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="E96" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G96" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="97" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C97" s="1">
+        <v>109</v>
+      </c>
+      <c r="D97" s="9">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="E97" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G97" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="98" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C98" s="1">
+        <v>205</v>
+      </c>
+      <c r="D98" s="9">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E98" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G98" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="99" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C99" s="1">
+        <v>206</v>
+      </c>
+      <c r="D99" s="9">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E99" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G99" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="100" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C100" s="1">
+        <v>207</v>
+      </c>
+      <c r="D100" s="9">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="E100" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G100" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="101" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C101" s="1">
+        <v>208</v>
+      </c>
+      <c r="D101" s="9">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="E101" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G101" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="102" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C102" s="1">
+        <v>209</v>
+      </c>
+      <c r="D102" s="9">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="E102" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G102" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="103" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C103" s="1">
+        <v>305</v>
+      </c>
+      <c r="D103" s="9">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E103" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G103" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="104" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C104" s="1">
+        <v>306</v>
+      </c>
+      <c r="D104" s="9">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E104" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G104" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="105" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C105" s="1">
+        <v>307</v>
+      </c>
+      <c r="D105" s="9">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="E105" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G105" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="106" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C106" s="1">
+        <v>308</v>
+      </c>
+      <c r="D106" s="9">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="E106" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G106" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="107" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C107" s="1">
+        <v>309</v>
+      </c>
+      <c r="D107" s="9">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="E107" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G107" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="108" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C108" s="1">
+        <v>125</v>
+      </c>
+      <c r="D108" s="9">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E108" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G108" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="109" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C109" s="1">
+        <v>126</v>
+      </c>
+      <c r="D109" s="9">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E109" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G109" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="110" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C110" s="1">
+        <v>127</v>
+      </c>
+      <c r="D110" s="9">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="E110" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G110" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="111" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C111" s="1">
+        <v>128</v>
+      </c>
+      <c r="D111" s="9">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="E111" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G111" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="112" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C112" s="1">
+        <v>129</v>
+      </c>
+      <c r="D112" s="9">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="E112" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G112" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="113" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C113" s="1">
+        <v>225</v>
+      </c>
+      <c r="D113" s="9">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E113" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G113" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="114" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C114" s="1">
+        <v>226</v>
+      </c>
+      <c r="D114" s="9">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E114" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G114" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="115" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C115" s="1">
+        <v>227</v>
+      </c>
+      <c r="D115" s="9">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="E115" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G115" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="116" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C116" s="1">
+        <v>228</v>
+      </c>
+      <c r="D116" s="9">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="E116" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G116" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="117" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C117" s="1">
+        <v>229</v>
+      </c>
+      <c r="D117" s="9">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="E117" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G117" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="118" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C118" s="1">
+        <v>325</v>
+      </c>
+      <c r="D118" s="9">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E118" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G118" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="119" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C119" s="1">
+        <v>326</v>
+      </c>
+      <c r="D119" s="9">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E119" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G119" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="120" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C120" s="1">
+        <v>327</v>
+      </c>
+      <c r="D120" s="9">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="E120" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G120" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="121" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C121" s="1">
+        <v>328</v>
+      </c>
+      <c r="D121" s="9">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="E121" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G121" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="122" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C122" s="1">
+        <v>329</v>
+      </c>
+      <c r="D122" s="9">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="E122" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G122" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="123" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C123" s="1">
         <v>991</v>
       </c>
-      <c r="D82" s="9">
-        <f t="shared" si="0"/>
+      <c r="D123" s="9">
+        <f>VLOOKUP( MOD(C123,100), $I$15:$K$51, 3, FALSE )</f>
         <v>5</v>
       </c>
-      <c r="E82" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F82" s="20" t="s">
+      <c r="E123" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F123" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="G82" s="20" t="str">
-        <f t="shared" si="1"/>
+      <c r="G123" s="20" t="str">
+        <f t="shared" si="0"/>
         <v>generic  (5kW cap @ 40F)</v>
       </c>
-      <c r="H82" s="20"/>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C83" s="1">
+      <c r="H123" s="20"/>
+    </row>
+    <row r="124" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C124" s="1">
         <v>992</v>
       </c>
-      <c r="D83" s="9">
-        <f t="shared" si="0"/>
+      <c r="D124" s="9">
+        <f>VLOOKUP( MOD(C124,100), $I$15:$K$51, 3, FALSE )</f>
         <v>11</v>
       </c>
-      <c r="E83" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F83" t="s">
+      <c r="E124" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F124" t="s">
         <v>79</v>
       </c>
-      <c r="G83" t="str">
-        <f t="shared" si="1"/>
+      <c r="G124" t="str">
+        <f t="shared" si="0"/>
         <v>generic  (11kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C84" s="1">
+    <row r="125" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C125" s="1">
         <v>993</v>
       </c>
-      <c r="D84" s="9">
-        <f t="shared" si="0"/>
+      <c r="D125" s="9">
+        <f>VLOOKUP( MOD(C125,100), $I$15:$K$51, 3, FALSE )</f>
         <v>20</v>
       </c>
-      <c r="E84" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F84" t="s">
+      <c r="E125" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F125" t="s">
         <v>79</v>
       </c>
-      <c r="G84" t="str">
-        <f t="shared" si="1"/>
+      <c r="G125" t="str">
+        <f t="shared" si="0"/>
         <v>generic  (20kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C85" s="1">
+    <row r="126" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C126" s="1">
         <v>994</v>
       </c>
-      <c r="D85" s="9">
-        <f t="shared" si="0"/>
+      <c r="D126" s="9">
+        <f>VLOOKUP( MOD(C126,100), $I$15:$K$51, 3, FALSE )</f>
         <v>26</v>
       </c>
-      <c r="E85" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F85" t="s">
+      <c r="E126" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F126" t="s">
         <v>79</v>
       </c>
-      <c r="G85" t="str">
-        <f t="shared" si="1"/>
+      <c r="G126" t="str">
+        <f t="shared" si="0"/>
         <v>generic  (26kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C86" s="1">
+    <row r="127" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C127" s="1">
         <v>995</v>
       </c>
-      <c r="D86" s="9">
-        <f t="shared" si="0"/>
+      <c r="D127" s="9">
+        <f>VLOOKUP( MOD(C127,100), $I$15:$K$51, 3, FALSE )</f>
         <v>40</v>
       </c>
-      <c r="E86" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="E127" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F127" t="s">
         <v>79</v>
       </c>
-      <c r="G86" t="str">
-        <f t="shared" si="1"/>
+      <c r="G127" t="str">
+        <f t="shared" si="0"/>
         <v>generic  (40kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C87" s="1">
+    <row r="128" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C128" s="1">
         <v>996</v>
       </c>
-      <c r="D87" s="9">
-        <f t="shared" si="0"/>
+      <c r="D128" s="9">
+        <f>VLOOKUP( MOD(C128,100), $I$15:$K$51, 3, FALSE )</f>
         <v>45</v>
       </c>
-      <c r="E87" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="E128" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F128" t="s">
         <v>79</v>
       </c>
-      <c r="G87" t="str">
-        <f t="shared" si="1"/>
+      <c r="G128" t="str">
+        <f t="shared" si="0"/>
         <v>generic  (45kW cap @ 40F)</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C88" s="17" t="s">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C129" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D88" s="18">
-        <v>0</v>
-      </c>
-      <c r="E88" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F88" t="s">
+      <c r="D129" s="18">
+        <v>0</v>
+      </c>
+      <c r="E129" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F129" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>